<commit_message>
Review tài liêu phân tích
</commit_message>
<xml_diff>
--- a/2018/Thao Phuong/01 QL DonVi-ChiNhanh/CIF1120_Danh muc don vi.xlsx
+++ b/2018/Thao Phuong/01 QL DonVi-ChiNhanh/CIF1120_Danh muc don vi.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Phuong\Analyze\Phương\Done\01 QL DonVi-ChiNhanh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SVN\THUCTAP\Thao Phuong\01 QL DonVi-ChiNhanh\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17715" windowHeight="8970" tabRatio="836" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17715" windowHeight="8970" tabRatio="836"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <definedName name="項目No">#REF!</definedName>
     <definedName name="項目名">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -471,6 +471,7 @@
   <authors>
     <author>Le Thi Thu Hien</author>
     <author>vinhphong</author>
+    <author>Phan Thanh Hoàng Vũ</author>
   </authors>
   <commentList>
     <comment ref="C4" authorId="0" shapeId="0">
@@ -753,6 +754,78 @@
         </r>
       </text>
     </comment>
+    <comment ref="K6" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Các control thiếu xử lý I hoặc O hoặc I/O</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O12" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Combo load từ bảng hiển thị 2 cột ID và Name
+Sau khi chọn fill vào combo là Name
+và truyền ID để search dữ liệu
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O13" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Thiếu xử lý combo câu SQL load ngầm là 2 cột ID và Name 
+Hiển thị ra combo là 1 cột Name
+Tuyền ID để search dữ liệu
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -835,6 +908,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>binhminh</author>
+    <author>Phan Thanh Hoàng Vũ</author>
   </authors>
   <commentList>
     <comment ref="C4" authorId="0" shapeId="0">
@@ -876,6 +950,50 @@
         </r>
       </text>
     </comment>
+    <comment ref="C5" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Nếu truyền @APK thì xử lý này là gọi đến màn hình xem chi tiết, không phải thêm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Nếu truyền tham số @DivisionID thì đây là xử lý thêm không phải là xử lý xem</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -885,6 +1003,7 @@
   <authors>
     <author>vinhphong</author>
     <author>Le Thi Thu Hien</author>
+    <author>Phan Thanh Hoàng Vũ</author>
   </authors>
   <commentList>
     <comment ref="D4" authorId="0" shapeId="0">
@@ -1003,6 +1122,77 @@
         </r>
       </text>
     </comment>
+    <comment ref="G5" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Dữ liệu load combo nếu truy xuất từ bảng Danh mục thì phải lấy ra ID và Name, hiện tại chỉ mới lấy Name
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Chưa đúng quy tắc đặt tên Store phải đặt CIP1120
+Đơn vị không có xử lý dùng chung nên Store search không có điều kiện search  là @@@</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Chưa đặt đúng quy tắc store, phải đặt CIP1121
+Store khi xóa thì chưa check  input đã bị sử dụng
+Store khi xóa chỉ xóa bảng AT1101 còn xóa bảng nào nữa không?
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1012,6 +1202,7 @@
   <authors>
     <author>vinhphong</author>
     <author>binhminh</author>
+    <author>Phan Thanh Hoàng Vũ</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0">
@@ -1226,6 +1417,72 @@
         </r>
       </text>
     </comment>
+    <comment ref="B24" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Đây là màn hình khai báo [Đơn vị] nên khi thêm không cần truyền tham số</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Khi xóa truyền tham số bị tiếu DivisionID</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Phan Thanh Hoàng Vũ:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Đối với ERP9 thì khi truyền tham số để gọi màn hình xem thì phải truyền APK.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -2122,13 +2379,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2246,6 +2503,17 @@
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="14">
@@ -2506,7 +2774,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2829,6 +3097,18 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2928,18 +3208,33 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2957,6 +3252,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3033,15 +3337,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>85877</xdr:colOff>
+          <xdr:colOff>85725</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>81643</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>2245179</xdr:colOff>
+          <xdr:colOff>2247900</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>81642</xdr:rowOff>
+          <xdr:rowOff>85725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3049,6 +3353,9 @@
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s5145"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3069,23 +3376,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -3215,6 +3509,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3250,6 +3561,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3428,8 +3756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J1:J2"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -3445,10 +3773,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
+      <c r="B1" s="143"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -3475,8 +3803,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -3515,14 +3843,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="138" t="s">
+      <c r="E4" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
     </row>
     <row r="5" spans="1:10" ht="11.25">
       <c r="A5" s="40">
@@ -3537,14 +3865,14 @@
       <c r="D5" s="99" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="139" t="s">
+      <c r="E5" s="145" t="s">
         <v>135</v>
       </c>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="130"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
     </row>
     <row r="6" spans="1:10" ht="12.75">
       <c r="A6" s="89">
@@ -3555,12 +3883,12 @@
       </c>
       <c r="C6" s="76"/>
       <c r="D6" s="65"/>
-      <c r="E6" s="140"/>
-      <c r="F6" s="141"/>
-      <c r="G6" s="141"/>
-      <c r="H6" s="141"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="142"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="147"/>
+      <c r="J6" s="148"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
       <c r="A7" s="90">
@@ -3571,12 +3899,12 @@
       </c>
       <c r="C7" s="77"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="132"/>
-      <c r="J7" s="133"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="139"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="91">
@@ -3587,12 +3915,12 @@
       </c>
       <c r="C8" s="77"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="134"/>
-      <c r="F8" s="135"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="136"/>
+      <c r="E8" s="140"/>
+      <c r="F8" s="141"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="142"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="92">
@@ -3603,12 +3931,12 @@
       </c>
       <c r="C9" s="77"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="133"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="139"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="93">
@@ -3619,12 +3947,12 @@
       </c>
       <c r="C10" s="77"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="133"/>
+      <c r="E10" s="137"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="139"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="94">
@@ -3635,12 +3963,12 @@
       </c>
       <c r="C11" s="77"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="132"/>
-      <c r="J11" s="133"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="138"/>
+      <c r="J11" s="139"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="95">
@@ -3651,12 +3979,12 @@
       </c>
       <c r="C12" s="77"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
-      <c r="I12" s="132"/>
-      <c r="J12" s="133"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
+      <c r="J12" s="139"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="96">
@@ -3667,12 +3995,12 @@
       </c>
       <c r="C13" s="77"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="131"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="132"/>
-      <c r="H13" s="132"/>
-      <c r="I13" s="132"/>
-      <c r="J13" s="133"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="139"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="97">
@@ -3683,12 +4011,12 @@
       </c>
       <c r="C14" s="77"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="132"/>
-      <c r="J14" s="133"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="139"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="40">
@@ -3699,12 +4027,12 @@
       </c>
       <c r="C15" s="77"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="130"/>
-      <c r="G15" s="130"/>
-      <c r="H15" s="130"/>
-      <c r="I15" s="130"/>
-      <c r="J15" s="130"/>
+      <c r="E15" s="136"/>
+      <c r="F15" s="136"/>
+      <c r="G15" s="136"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="136"/>
+      <c r="J15" s="136"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="89">
@@ -3715,12 +4043,12 @@
       </c>
       <c r="C16" s="77"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="130"/>
-      <c r="F16" s="130"/>
-      <c r="G16" s="130"/>
-      <c r="H16" s="130"/>
-      <c r="I16" s="130"/>
-      <c r="J16" s="130"/>
+      <c r="E16" s="136"/>
+      <c r="F16" s="136"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="136"/>
+      <c r="J16" s="136"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="90">
@@ -3731,12 +4059,12 @@
       </c>
       <c r="C17" s="77"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="130"/>
-      <c r="F17" s="130"/>
-      <c r="G17" s="130"/>
-      <c r="H17" s="130"/>
-      <c r="I17" s="130"/>
-      <c r="J17" s="130"/>
+      <c r="E17" s="136"/>
+      <c r="F17" s="136"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="136"/>
+      <c r="J17" s="136"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="91">
@@ -3747,12 +4075,12 @@
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="130"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="130"/>
-      <c r="J18" s="130"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="136"/>
+      <c r="H18" s="136"/>
+      <c r="I18" s="136"/>
+      <c r="J18" s="136"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="92">
@@ -3763,12 +4091,12 @@
       </c>
       <c r="C19" s="77"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="130"/>
-      <c r="F19" s="130"/>
-      <c r="G19" s="130"/>
-      <c r="H19" s="130"/>
-      <c r="I19" s="130"/>
-      <c r="J19" s="130"/>
+      <c r="E19" s="136"/>
+      <c r="F19" s="136"/>
+      <c r="G19" s="136"/>
+      <c r="H19" s="136"/>
+      <c r="I19" s="136"/>
+      <c r="J19" s="136"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="93">
@@ -3779,12 +4107,12 @@
       </c>
       <c r="C20" s="77"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="130"/>
-      <c r="F20" s="130"/>
-      <c r="G20" s="130"/>
-      <c r="H20" s="130"/>
-      <c r="I20" s="130"/>
-      <c r="J20" s="130"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
+      <c r="G20" s="136"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="136"/>
+      <c r="J20" s="136"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="94">
@@ -3795,12 +4123,12 @@
       </c>
       <c r="C21" s="77"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="130"/>
-      <c r="F21" s="130"/>
-      <c r="G21" s="130"/>
-      <c r="H21" s="130"/>
-      <c r="I21" s="130"/>
-      <c r="J21" s="130"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
+      <c r="G21" s="136"/>
+      <c r="H21" s="136"/>
+      <c r="I21" s="136"/>
+      <c r="J21" s="136"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="95">
@@ -3811,12 +4139,12 @@
       </c>
       <c r="C22" s="77"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
-      <c r="G22" s="130"/>
-      <c r="H22" s="130"/>
-      <c r="I22" s="130"/>
-      <c r="J22" s="130"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="136"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="136"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="96">
@@ -3827,12 +4155,12 @@
       </c>
       <c r="C23" s="77"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
-      <c r="G23" s="130"/>
-      <c r="H23" s="130"/>
-      <c r="I23" s="130"/>
-      <c r="J23" s="130"/>
+      <c r="E23" s="136"/>
+      <c r="F23" s="136"/>
+      <c r="G23" s="136"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="136"/>
+      <c r="J23" s="136"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="97">
@@ -3843,12 +4171,12 @@
       </c>
       <c r="C24" s="77"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
-      <c r="G24" s="130"/>
-      <c r="H24" s="130"/>
-      <c r="I24" s="130"/>
-      <c r="J24" s="130"/>
+      <c r="E24" s="136"/>
+      <c r="F24" s="136"/>
+      <c r="G24" s="136"/>
+      <c r="H24" s="136"/>
+      <c r="I24" s="136"/>
+      <c r="J24" s="136"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="40">
@@ -3859,12 +4187,12 @@
       </c>
       <c r="C25" s="77"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="130"/>
-      <c r="G25" s="130"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="130"/>
-      <c r="J25" s="130"/>
+      <c r="E25" s="136"/>
+      <c r="F25" s="136"/>
+      <c r="G25" s="136"/>
+      <c r="H25" s="136"/>
+      <c r="I25" s="136"/>
+      <c r="J25" s="136"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="40">
@@ -3875,12 +4203,12 @@
       </c>
       <c r="C26" s="77"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="130"/>
-      <c r="G26" s="130"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="130"/>
-      <c r="J26" s="130"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="89">
@@ -3891,12 +4219,12 @@
       </c>
       <c r="C27" s="77"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="130"/>
-      <c r="G27" s="130"/>
-      <c r="H27" s="130"/>
-      <c r="I27" s="130"/>
-      <c r="J27" s="130"/>
+      <c r="E27" s="136"/>
+      <c r="F27" s="136"/>
+      <c r="G27" s="136"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="136"/>
+      <c r="J27" s="136"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="90">
@@ -3907,12 +4235,12 @@
       </c>
       <c r="C28" s="77"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="130"/>
-      <c r="F28" s="130"/>
-      <c r="G28" s="130"/>
-      <c r="H28" s="130"/>
-      <c r="I28" s="130"/>
-      <c r="J28" s="130"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="136"/>
+      <c r="G28" s="136"/>
+      <c r="H28" s="136"/>
+      <c r="I28" s="136"/>
+      <c r="J28" s="136"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="91">
@@ -3923,12 +4251,12 @@
       </c>
       <c r="C29" s="77"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="130"/>
-      <c r="F29" s="130"/>
-      <c r="G29" s="130"/>
-      <c r="H29" s="130"/>
-      <c r="I29" s="130"/>
-      <c r="J29" s="130"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
+      <c r="G29" s="136"/>
+      <c r="H29" s="136"/>
+      <c r="I29" s="136"/>
+      <c r="J29" s="136"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="92">
@@ -3939,12 +4267,12 @@
       </c>
       <c r="C30" s="77"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="130"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="130"/>
-      <c r="I30" s="130"/>
-      <c r="J30" s="130"/>
+      <c r="E30" s="136"/>
+      <c r="F30" s="136"/>
+      <c r="G30" s="136"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="136"/>
+      <c r="J30" s="136"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="93">
@@ -3955,12 +4283,12 @@
       </c>
       <c r="C31" s="77"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="130"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
-      <c r="I31" s="130"/>
-      <c r="J31" s="130"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="136"/>
+      <c r="I31" s="136"/>
+      <c r="J31" s="136"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="94">
@@ -3971,12 +4299,12 @@
       </c>
       <c r="C32" s="77"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="130"/>
-      <c r="F32" s="130"/>
-      <c r="G32" s="130"/>
-      <c r="H32" s="130"/>
-      <c r="I32" s="130"/>
-      <c r="J32" s="130"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="136"/>
+      <c r="G32" s="136"/>
+      <c r="H32" s="136"/>
+      <c r="I32" s="136"/>
+      <c r="J32" s="136"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="95">
@@ -3987,12 +4315,12 @@
       </c>
       <c r="C33" s="77"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="130"/>
-      <c r="F33" s="130"/>
-      <c r="G33" s="130"/>
-      <c r="H33" s="130"/>
-      <c r="I33" s="130"/>
-      <c r="J33" s="130"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="136"/>
+      <c r="G33" s="136"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="136"/>
+      <c r="J33" s="136"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="96">
@@ -4003,12 +4331,12 @@
       </c>
       <c r="C34" s="77"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="130"/>
-      <c r="F34" s="130"/>
-      <c r="G34" s="130"/>
-      <c r="H34" s="130"/>
-      <c r="I34" s="130"/>
-      <c r="J34" s="130"/>
+      <c r="E34" s="136"/>
+      <c r="F34" s="136"/>
+      <c r="G34" s="136"/>
+      <c r="H34" s="136"/>
+      <c r="I34" s="136"/>
+      <c r="J34" s="136"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="97">
@@ -4019,12 +4347,12 @@
       </c>
       <c r="C35" s="77"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="130"/>
-      <c r="G35" s="130"/>
-      <c r="H35" s="130"/>
-      <c r="I35" s="130"/>
-      <c r="J35" s="130"/>
+      <c r="E35" s="136"/>
+      <c r="F35" s="136"/>
+      <c r="G35" s="136"/>
+      <c r="H35" s="136"/>
+      <c r="I35" s="136"/>
+      <c r="J35" s="136"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="40">
@@ -4035,12 +4363,12 @@
       </c>
       <c r="C36" s="77"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="130"/>
-      <c r="G36" s="130"/>
-      <c r="H36" s="130"/>
-      <c r="I36" s="130"/>
-      <c r="J36" s="130"/>
+      <c r="E36" s="136"/>
+      <c r="F36" s="136"/>
+      <c r="G36" s="136"/>
+      <c r="H36" s="136"/>
+      <c r="I36" s="136"/>
+      <c r="J36" s="136"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="89">
@@ -4051,12 +4379,12 @@
       </c>
       <c r="C37" s="77"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="130"/>
-      <c r="F37" s="130"/>
-      <c r="G37" s="130"/>
-      <c r="H37" s="130"/>
-      <c r="I37" s="130"/>
-      <c r="J37" s="130"/>
+      <c r="E37" s="136"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="136"/>
+      <c r="H37" s="136"/>
+      <c r="I37" s="136"/>
+      <c r="J37" s="136"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="90">
@@ -4067,12 +4395,12 @@
       </c>
       <c r="C38" s="77"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="130"/>
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="130"/>
-      <c r="I38" s="130"/>
-      <c r="J38" s="130"/>
+      <c r="E38" s="136"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="136"/>
+      <c r="H38" s="136"/>
+      <c r="I38" s="136"/>
+      <c r="J38" s="136"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="91">
@@ -4083,12 +4411,12 @@
       </c>
       <c r="C39" s="77"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="130"/>
-      <c r="F39" s="130"/>
-      <c r="G39" s="130"/>
-      <c r="H39" s="130"/>
-      <c r="I39" s="130"/>
-      <c r="J39" s="130"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="136"/>
+      <c r="G39" s="136"/>
+      <c r="H39" s="136"/>
+      <c r="I39" s="136"/>
+      <c r="J39" s="136"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="92">
@@ -4099,12 +4427,12 @@
       </c>
       <c r="C40" s="77"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="130"/>
-      <c r="F40" s="130"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="130"/>
-      <c r="I40" s="130"/>
-      <c r="J40" s="130"/>
+      <c r="E40" s="136"/>
+      <c r="F40" s="136"/>
+      <c r="G40" s="136"/>
+      <c r="H40" s="136"/>
+      <c r="I40" s="136"/>
+      <c r="J40" s="136"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="93">
@@ -4115,12 +4443,12 @@
       </c>
       <c r="C41" s="77"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="130"/>
-      <c r="G41" s="130"/>
-      <c r="H41" s="130"/>
-      <c r="I41" s="130"/>
-      <c r="J41" s="130"/>
+      <c r="E41" s="136"/>
+      <c r="F41" s="136"/>
+      <c r="G41" s="136"/>
+      <c r="H41" s="136"/>
+      <c r="I41" s="136"/>
+      <c r="J41" s="136"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="94">
@@ -4131,12 +4459,12 @@
       </c>
       <c r="C42" s="77"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="130"/>
-      <c r="G42" s="130"/>
-      <c r="H42" s="130"/>
-      <c r="I42" s="130"/>
-      <c r="J42" s="130"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="136"/>
+      <c r="G42" s="136"/>
+      <c r="H42" s="136"/>
+      <c r="I42" s="136"/>
+      <c r="J42" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="40">
@@ -4204,8 +4532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView view="pageBreakPreview" zoomScale="84" zoomScaleSheetLayoutView="84" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -4223,10 +4551,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
+      <c r="B1" s="143"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -4257,8 +4585,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -4289,20 +4617,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="12" customHeight="1">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="149" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="145"/>
-      <c r="C4" s="145"/>
-      <c r="D4" s="145"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="145"/>
-      <c r="H4" s="144"/>
-      <c r="I4" s="143" t="s">
+      <c r="B4" s="151"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="150"/>
+      <c r="I4" s="149" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="144"/>
+      <c r="J4" s="150"/>
     </row>
     <row r="5" spans="1:10" ht="12" customHeight="1">
       <c r="A5" s="42"/>
@@ -4313,10 +4641,10 @@
       <c r="F5" s="43"/>
       <c r="G5" s="43"/>
       <c r="H5" s="44"/>
-      <c r="I5" s="152" t="s">
+      <c r="I5" s="158" t="s">
         <v>136</v>
       </c>
-      <c r="J5" s="153"/>
+      <c r="J5" s="159"/>
     </row>
     <row r="6" spans="1:10" ht="12" customHeight="1">
       <c r="A6" s="42"/>
@@ -4327,8 +4655,8 @@
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
       <c r="H6" s="45"/>
-      <c r="I6" s="154"/>
-      <c r="J6" s="155"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="161"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
       <c r="A7" s="42"/>
@@ -4339,8 +4667,8 @@
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="45"/>
-      <c r="I7" s="154"/>
-      <c r="J7" s="155"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="161"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="42"/>
@@ -4351,8 +4679,8 @@
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
       <c r="H8" s="45"/>
-      <c r="I8" s="154"/>
-      <c r="J8" s="155"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="161"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="42"/>
@@ -4363,8 +4691,8 @@
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
       <c r="H9" s="45"/>
-      <c r="I9" s="154"/>
-      <c r="J9" s="155"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="161"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="42"/>
@@ -4375,8 +4703,8 @@
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="45"/>
-      <c r="I10" s="156"/>
-      <c r="J10" s="157"/>
+      <c r="I10" s="162"/>
+      <c r="J10" s="163"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="42"/>
@@ -4387,10 +4715,10 @@
       <c r="F11" s="43"/>
       <c r="G11" s="43"/>
       <c r="H11" s="46"/>
-      <c r="I11" s="143" t="s">
+      <c r="I11" s="149" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="144"/>
+      <c r="J11" s="150"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="42"/>
@@ -4401,10 +4729,10 @@
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
       <c r="H12" s="45"/>
-      <c r="I12" s="146" t="s">
+      <c r="I12" s="152" t="s">
         <v>137</v>
       </c>
-      <c r="J12" s="147"/>
+      <c r="J12" s="153"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="42"/>
@@ -4415,8 +4743,8 @@
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
       <c r="H13" s="45"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="149"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="155"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="42"/>
@@ -4427,8 +4755,8 @@
       <c r="F14" s="43"/>
       <c r="G14" s="43"/>
       <c r="H14" s="45"/>
-      <c r="I14" s="148"/>
-      <c r="J14" s="149"/>
+      <c r="I14" s="154"/>
+      <c r="J14" s="155"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="42"/>
@@ -4439,8 +4767,8 @@
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
       <c r="H15" s="45"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="149"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="155"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="42"/>
@@ -4451,8 +4779,8 @@
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
       <c r="H16" s="45"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="149"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="155"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="42"/>
@@ -4463,8 +4791,8 @@
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
       <c r="H17" s="45"/>
-      <c r="I17" s="148"/>
-      <c r="J17" s="149"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="155"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="42"/>
@@ -4475,8 +4803,8 @@
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
       <c r="H18" s="45"/>
-      <c r="I18" s="148"/>
-      <c r="J18" s="149"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="155"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="42"/>
@@ -4487,8 +4815,8 @@
       <c r="F19" s="43"/>
       <c r="G19" s="43"/>
       <c r="H19" s="45"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="149"/>
+      <c r="I19" s="154"/>
+      <c r="J19" s="155"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="42"/>
@@ -4499,8 +4827,8 @@
       <c r="F20" s="43"/>
       <c r="G20" s="43"/>
       <c r="H20" s="45"/>
-      <c r="I20" s="148"/>
-      <c r="J20" s="149"/>
+      <c r="I20" s="154"/>
+      <c r="J20" s="155"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="42"/>
@@ -4511,8 +4839,8 @@
       <c r="F21" s="43"/>
       <c r="G21" s="43"/>
       <c r="H21" s="45"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="149"/>
+      <c r="I21" s="154"/>
+      <c r="J21" s="155"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="42"/>
@@ -4523,8 +4851,8 @@
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
       <c r="H22" s="45"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="149"/>
+      <c r="I22" s="154"/>
+      <c r="J22" s="155"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="42"/>
@@ -4535,8 +4863,8 @@
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
       <c r="H23" s="45"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="149"/>
+      <c r="I23" s="154"/>
+      <c r="J23" s="155"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="42"/>
@@ -4547,8 +4875,8 @@
       <c r="F24" s="43"/>
       <c r="G24" s="43"/>
       <c r="H24" s="45"/>
-      <c r="I24" s="148"/>
-      <c r="J24" s="149"/>
+      <c r="I24" s="154"/>
+      <c r="J24" s="155"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="42"/>
@@ -4559,8 +4887,8 @@
       <c r="F25" s="43"/>
       <c r="G25" s="43"/>
       <c r="H25" s="45"/>
-      <c r="I25" s="148"/>
-      <c r="J25" s="149"/>
+      <c r="I25" s="154"/>
+      <c r="J25" s="155"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="42"/>
@@ -4571,8 +4899,8 @@
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
       <c r="H26" s="45"/>
-      <c r="I26" s="148"/>
-      <c r="J26" s="149"/>
+      <c r="I26" s="154"/>
+      <c r="J26" s="155"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="42"/>
@@ -4583,8 +4911,8 @@
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
       <c r="H27" s="45"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="149"/>
+      <c r="I27" s="154"/>
+      <c r="J27" s="155"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="42"/>
@@ -4595,8 +4923,8 @@
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
       <c r="H28" s="45"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="149"/>
+      <c r="I28" s="154"/>
+      <c r="J28" s="155"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="42"/>
@@ -4607,8 +4935,8 @@
       <c r="F29" s="43"/>
       <c r="G29" s="43"/>
       <c r="H29" s="45"/>
-      <c r="I29" s="148"/>
-      <c r="J29" s="149"/>
+      <c r="I29" s="154"/>
+      <c r="J29" s="155"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="42"/>
@@ -4619,8 +4947,8 @@
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
       <c r="H30" s="45"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="149"/>
+      <c r="I30" s="154"/>
+      <c r="J30" s="155"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="42"/>
@@ -4631,8 +4959,8 @@
       <c r="F31" s="43"/>
       <c r="G31" s="43"/>
       <c r="H31" s="45"/>
-      <c r="I31" s="148"/>
-      <c r="J31" s="149"/>
+      <c r="I31" s="154"/>
+      <c r="J31" s="155"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="42"/>
@@ -4643,8 +4971,8 @@
       <c r="F32" s="43"/>
       <c r="G32" s="43"/>
       <c r="H32" s="45"/>
-      <c r="I32" s="148"/>
-      <c r="J32" s="149"/>
+      <c r="I32" s="154"/>
+      <c r="J32" s="155"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="42"/>
@@ -4655,8 +4983,8 @@
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
       <c r="H33" s="45"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="149"/>
+      <c r="I33" s="154"/>
+      <c r="J33" s="155"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="42"/>
@@ -4667,8 +4995,8 @@
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
       <c r="H34" s="45"/>
-      <c r="I34" s="148"/>
-      <c r="J34" s="149"/>
+      <c r="I34" s="154"/>
+      <c r="J34" s="155"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="42"/>
@@ -4679,8 +5007,8 @@
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
       <c r="H35" s="45"/>
-      <c r="I35" s="148"/>
-      <c r="J35" s="149"/>
+      <c r="I35" s="154"/>
+      <c r="J35" s="155"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="42"/>
@@ -4691,8 +5019,8 @@
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
       <c r="H36" s="45"/>
-      <c r="I36" s="148"/>
-      <c r="J36" s="149"/>
+      <c r="I36" s="154"/>
+      <c r="J36" s="155"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="42"/>
@@ -4703,8 +5031,8 @@
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
       <c r="H37" s="45"/>
-      <c r="I37" s="148"/>
-      <c r="J37" s="149"/>
+      <c r="I37" s="154"/>
+      <c r="J37" s="155"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="42"/>
@@ -4715,8 +5043,8 @@
       <c r="F38" s="43"/>
       <c r="G38" s="43"/>
       <c r="H38" s="45"/>
-      <c r="I38" s="148"/>
-      <c r="J38" s="149"/>
+      <c r="I38" s="154"/>
+      <c r="J38" s="155"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="42"/>
@@ -4727,8 +5055,8 @@
       <c r="F39" s="43"/>
       <c r="G39" s="43"/>
       <c r="H39" s="45"/>
-      <c r="I39" s="148"/>
-      <c r="J39" s="149"/>
+      <c r="I39" s="154"/>
+      <c r="J39" s="155"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="42"/>
@@ -4739,8 +5067,8 @@
       <c r="F40" s="43"/>
       <c r="G40" s="43"/>
       <c r="H40" s="45"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="149"/>
+      <c r="I40" s="154"/>
+      <c r="J40" s="155"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="42"/>
@@ -4751,8 +5079,8 @@
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
       <c r="H41" s="45"/>
-      <c r="I41" s="148"/>
-      <c r="J41" s="149"/>
+      <c r="I41" s="154"/>
+      <c r="J41" s="155"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="42"/>
@@ -4763,8 +5091,8 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
       <c r="H42" s="45"/>
-      <c r="I42" s="148"/>
-      <c r="J42" s="149"/>
+      <c r="I42" s="154"/>
+      <c r="J42" s="155"/>
     </row>
     <row r="43" spans="1:10" ht="12" customHeight="1">
       <c r="A43" s="47"/>
@@ -4775,8 +5103,8 @@
       <c r="F43" s="48"/>
       <c r="G43" s="48"/>
       <c r="H43" s="49"/>
-      <c r="I43" s="150"/>
-      <c r="J43" s="151"/>
+      <c r="I43" s="156"/>
+      <c r="J43" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4833,11 +5161,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -4861,12 +5189,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="30" t="s">
         <v>1</v>
       </c>
@@ -4874,16 +5202,16 @@
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="G1" s="158" t="s">
+      <c r="G1" s="164" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="159"/>
-      <c r="I1" s="160" t="str">
+      <c r="H1" s="165"/>
+      <c r="I1" s="166" t="str">
         <f>'Update History'!$F$1</f>
         <v>CIF1120</v>
       </c>
-      <c r="J1" s="161"/>
-      <c r="K1" s="162"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="168"/>
       <c r="L1" s="31" t="s">
         <v>5</v>
       </c>
@@ -4900,10 +5228,10 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
       <c r="E2" s="30" t="s">
         <v>2</v>
       </c>
@@ -4911,16 +5239,16 @@
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
       </c>
-      <c r="G2" s="158" t="s">
+      <c r="G2" s="164" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="159"/>
-      <c r="I2" s="160" t="str">
+      <c r="H2" s="165"/>
+      <c r="I2" s="166" t="str">
         <f>'Update History'!F2</f>
         <v>Danh mục đơn vị</v>
       </c>
-      <c r="J2" s="161"/>
-      <c r="K2" s="162"/>
+      <c r="J2" s="167"/>
+      <c r="K2" s="168"/>
       <c r="L2" s="31" t="s">
         <v>6</v>
       </c>
@@ -5041,7 +5369,7 @@
       </c>
       <c r="I6" s="62"/>
       <c r="J6" s="62"/>
-      <c r="K6" s="40"/>
+      <c r="K6" s="130"/>
       <c r="L6" s="69"/>
       <c r="M6" s="69"/>
       <c r="N6" s="69"/>
@@ -5074,7 +5402,7 @@
       </c>
       <c r="I7" s="62"/>
       <c r="J7" s="62"/>
-      <c r="K7" s="40"/>
+      <c r="K7" s="130"/>
       <c r="L7" s="86"/>
       <c r="M7" s="86"/>
       <c r="N7" s="86"/>
@@ -5107,7 +5435,7 @@
       </c>
       <c r="I8" s="62"/>
       <c r="J8" s="62"/>
-      <c r="K8" s="40"/>
+      <c r="K8" s="130"/>
       <c r="L8" s="69"/>
       <c r="M8" s="69"/>
       <c r="N8" s="69"/>
@@ -5140,7 +5468,7 @@
       </c>
       <c r="I9" s="62"/>
       <c r="J9" s="62"/>
-      <c r="K9" s="40"/>
+      <c r="K9" s="130"/>
       <c r="L9" s="86"/>
       <c r="M9" s="86"/>
       <c r="N9" s="86"/>
@@ -5173,7 +5501,7 @@
       </c>
       <c r="I10" s="62"/>
       <c r="J10" s="62"/>
-      <c r="K10" s="40"/>
+      <c r="K10" s="130"/>
       <c r="L10" s="69"/>
       <c r="M10" s="69"/>
       <c r="N10" s="69"/>
@@ -5206,7 +5534,7 @@
       </c>
       <c r="I11" s="62"/>
       <c r="J11" s="62"/>
-      <c r="K11" s="40"/>
+      <c r="K11" s="130"/>
       <c r="L11" s="81"/>
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
@@ -5239,11 +5567,11 @@
       </c>
       <c r="I12" s="62"/>
       <c r="J12" s="62"/>
-      <c r="K12" s="40"/>
+      <c r="K12" s="130"/>
       <c r="L12" s="88"/>
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
-      <c r="O12" s="86"/>
+      <c r="O12" s="131"/>
     </row>
     <row r="13" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -5272,11 +5600,11 @@
       </c>
       <c r="I13" s="62"/>
       <c r="J13" s="62"/>
-      <c r="K13" s="40"/>
+      <c r="K13" s="130"/>
       <c r="L13" s="88"/>
       <c r="M13" s="69"/>
       <c r="N13" s="69"/>
-      <c r="O13" s="86"/>
+      <c r="O13" s="131"/>
     </row>
     <row r="14" spans="1:15" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -5301,7 +5629,7 @@
       <c r="H14" s="40"/>
       <c r="I14" s="62"/>
       <c r="J14" s="62"/>
-      <c r="K14" s="40"/>
+      <c r="K14" s="130"/>
       <c r="L14" s="62"/>
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
@@ -5330,7 +5658,7 @@
       <c r="H15" s="40"/>
       <c r="I15" s="62"/>
       <c r="J15" s="62"/>
-      <c r="K15" s="40"/>
+      <c r="K15" s="130"/>
       <c r="L15" s="62"/>
       <c r="M15" s="69"/>
       <c r="N15" s="69"/>
@@ -5359,7 +5687,7 @@
       <c r="H16" s="40"/>
       <c r="I16" s="62"/>
       <c r="J16" s="62"/>
-      <c r="K16" s="40"/>
+      <c r="K16" s="130"/>
       <c r="L16" s="62"/>
       <c r="M16" s="69"/>
       <c r="N16" s="69"/>
@@ -5388,7 +5716,7 @@
       <c r="H17" s="40"/>
       <c r="I17" s="62"/>
       <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
+      <c r="K17" s="130"/>
       <c r="L17" s="69"/>
       <c r="M17" s="69"/>
       <c r="N17" s="69"/>
@@ -5421,7 +5749,7 @@
       </c>
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
+      <c r="K18" s="130"/>
       <c r="L18" s="40"/>
       <c r="M18" s="40"/>
       <c r="N18" s="69"/>
@@ -5454,7 +5782,7 @@
       </c>
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
+      <c r="K19" s="130"/>
       <c r="L19" s="40"/>
       <c r="M19" s="40"/>
       <c r="N19" s="81"/>
@@ -5487,7 +5815,7 @@
       </c>
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
+      <c r="K20" s="130"/>
       <c r="L20" s="40"/>
       <c r="M20" s="40"/>
       <c r="N20" s="69"/>
@@ -5520,7 +5848,7 @@
       </c>
       <c r="I21" s="40"/>
       <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
+      <c r="K21" s="130"/>
       <c r="L21" s="40"/>
       <c r="M21" s="40"/>
       <c r="N21" s="69"/>
@@ -5553,7 +5881,7 @@
       </c>
       <c r="I22" s="40"/>
       <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
+      <c r="K22" s="130"/>
       <c r="L22" s="40"/>
       <c r="M22" s="40"/>
       <c r="N22" s="86"/>
@@ -5586,7 +5914,7 @@
       </c>
       <c r="I23" s="40"/>
       <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
+      <c r="K23" s="130"/>
       <c r="L23" s="40"/>
       <c r="M23" s="40"/>
       <c r="N23" s="69"/>
@@ -5619,7 +5947,7 @@
       </c>
       <c r="I24" s="40"/>
       <c r="J24" s="61"/>
-      <c r="K24" s="40"/>
+      <c r="K24" s="130"/>
       <c r="L24" s="61"/>
       <c r="M24" s="61"/>
       <c r="N24" s="40"/>
@@ -5652,7 +5980,7 @@
       </c>
       <c r="I25" s="40"/>
       <c r="J25" s="61"/>
-      <c r="K25" s="40"/>
+      <c r="K25" s="130"/>
       <c r="L25" s="62"/>
       <c r="M25" s="61"/>
       <c r="N25" s="61"/>
@@ -7211,7 +7539,7 @@
   <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+      <selection activeCell="F18" sqref="F18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -7235,7 +7563,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="171" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="113"/>
@@ -7271,7 +7599,7 @@
       <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="166"/>
+      <c r="A2" s="172"/>
       <c r="B2" s="114"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
@@ -7320,15 +7648,15 @@
       <c r="E4" s="100" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="137" t="s">
+      <c r="F4" s="143" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137" t="s">
+      <c r="G4" s="143"/>
+      <c r="H4" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="137"/>
-      <c r="J4" s="137"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
     </row>
     <row r="5" spans="1:12" s="34" customFormat="1" ht="24.75" customHeight="1">
       <c r="A5" s="33">
@@ -7337,22 +7665,22 @@
       <c r="B5" s="115" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="115" t="s">
+      <c r="C5" s="132" t="s">
         <v>182</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="F5" s="163" t="s">
+      <c r="F5" s="169" t="s">
         <v>183</v>
       </c>
-      <c r="G5" s="164"/>
-      <c r="H5" s="167" t="s">
+      <c r="G5" s="170"/>
+      <c r="H5" s="173" t="s">
         <v>187</v>
       </c>
-      <c r="I5" s="168"/>
-      <c r="J5" s="169"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="175"/>
     </row>
     <row r="6" spans="1:12" s="34" customFormat="1" ht="39.75" customHeight="1">
       <c r="A6" s="33">
@@ -7361,22 +7689,22 @@
       <c r="B6" s="115" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="132" t="s">
         <v>184</v>
       </c>
       <c r="D6" s="33"/>
       <c r="E6" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="F6" s="163" t="s">
+      <c r="F6" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="G6" s="164"/>
-      <c r="H6" s="167" t="s">
+      <c r="G6" s="170"/>
+      <c r="H6" s="173" t="s">
         <v>185</v>
       </c>
-      <c r="I6" s="168"/>
-      <c r="J6" s="169"/>
+      <c r="I6" s="174"/>
+      <c r="J6" s="175"/>
     </row>
     <row r="7" spans="1:12" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A7" s="33">
@@ -7386,11 +7714,11 @@
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
-      <c r="H7" s="167"/>
-      <c r="I7" s="168"/>
-      <c r="J7" s="169"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="178"/>
+      <c r="I7" s="179"/>
+      <c r="J7" s="180"/>
     </row>
     <row r="8" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="33">
@@ -7400,11 +7728,11 @@
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
-      <c r="H8" s="167"/>
-      <c r="I8" s="168"/>
-      <c r="J8" s="169"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="177"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="180"/>
     </row>
     <row r="9" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="33">
@@ -7414,11 +7742,11 @@
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="32"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="168"/>
-      <c r="J9" s="169"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="180"/>
     </row>
     <row r="10" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="33">
@@ -7428,11 +7756,11 @@
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="164"/>
-      <c r="H10" s="167"/>
-      <c r="I10" s="168"/>
-      <c r="J10" s="169"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="179"/>
+      <c r="J10" s="180"/>
     </row>
     <row r="11" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="33">
@@ -7442,11 +7770,11 @@
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="163"/>
-      <c r="G11" s="164"/>
-      <c r="H11" s="167"/>
-      <c r="I11" s="168"/>
-      <c r="J11" s="169"/>
+      <c r="F11" s="176"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="178"/>
+      <c r="I11" s="179"/>
+      <c r="J11" s="180"/>
     </row>
     <row r="12" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="33">
@@ -7456,11 +7784,11 @@
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="163"/>
-      <c r="G12" s="164"/>
-      <c r="H12" s="167"/>
-      <c r="I12" s="168"/>
-      <c r="J12" s="169"/>
+      <c r="F12" s="176"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="180"/>
     </row>
     <row r="13" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -7470,11 +7798,11 @@
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="164"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="168"/>
-      <c r="J13" s="169"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="179"/>
+      <c r="J13" s="180"/>
     </row>
     <row r="14" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -7484,11 +7812,11 @@
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="164"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="168"/>
-      <c r="J14" s="169"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="179"/>
+      <c r="J14" s="180"/>
     </row>
     <row r="15" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -7498,11 +7826,11 @@
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="163"/>
-      <c r="G15" s="164"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="168"/>
-      <c r="J15" s="169"/>
+      <c r="F15" s="176"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="179"/>
+      <c r="J15" s="180"/>
     </row>
     <row r="16" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="33">
@@ -7512,11 +7840,11 @@
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="32"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="164"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="168"/>
-      <c r="J16" s="169"/>
+      <c r="F16" s="176"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="179"/>
+      <c r="J16" s="180"/>
     </row>
     <row r="17" spans="1:18" s="34" customFormat="1" ht="11.25">
       <c r="A17" s="33">
@@ -7526,11 +7854,11 @@
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="32"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="164"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="168"/>
-      <c r="J17" s="169"/>
+      <c r="F17" s="176"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="179"/>
+      <c r="J17" s="180"/>
     </row>
     <row r="18" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -7540,11 +7868,11 @@
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="32"/>
-      <c r="F18" s="163"/>
-      <c r="G18" s="164"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="168"/>
-      <c r="J18" s="169"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="178"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="180"/>
     </row>
     <row r="19" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -7554,11 +7882,11 @@
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="32"/>
-      <c r="F19" s="163"/>
-      <c r="G19" s="164"/>
-      <c r="H19" s="167"/>
-      <c r="I19" s="168"/>
-      <c r="J19" s="169"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="179"/>
+      <c r="J19" s="180"/>
     </row>
     <row r="20" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="33">
@@ -7568,11 +7896,11 @@
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="164"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="168"/>
-      <c r="J20" s="169"/>
+      <c r="F20" s="176"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="179"/>
+      <c r="J20" s="180"/>
     </row>
     <row r="21" spans="1:18" s="34" customFormat="1" ht="11.25">
       <c r="A21" s="33">
@@ -7582,11 +7910,11 @@
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="163"/>
-      <c r="G21" s="164"/>
-      <c r="H21" s="167"/>
-      <c r="I21" s="168"/>
-      <c r="J21" s="169"/>
+      <c r="F21" s="176"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="179"/>
+      <c r="J21" s="180"/>
     </row>
     <row r="22" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
@@ -7596,11 +7924,11 @@
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="32"/>
-      <c r="F22" s="131"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="167"/>
-      <c r="I22" s="168"/>
-      <c r="J22" s="169"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="179"/>
+      <c r="J22" s="180"/>
     </row>
     <row r="23" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
@@ -7610,11 +7938,11 @@
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
-      <c r="F23" s="131"/>
-      <c r="G23" s="133"/>
-      <c r="H23" s="167"/>
-      <c r="I23" s="168"/>
-      <c r="J23" s="169"/>
+      <c r="F23" s="137"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="179"/>
+      <c r="J23" s="180"/>
     </row>
     <row r="24" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
@@ -7624,11 +7952,11 @@
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="32"/>
-      <c r="F24" s="131"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="167"/>
-      <c r="I24" s="168"/>
-      <c r="J24" s="169"/>
+      <c r="F24" s="137"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="179"/>
+      <c r="J24" s="180"/>
     </row>
     <row r="25" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
@@ -7638,11 +7966,11 @@
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
-      <c r="F25" s="131"/>
-      <c r="G25" s="133"/>
-      <c r="H25" s="167"/>
-      <c r="I25" s="168"/>
-      <c r="J25" s="169"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="179"/>
+      <c r="J25" s="180"/>
     </row>
     <row r="26" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
@@ -7652,11 +7980,11 @@
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="131"/>
-      <c r="G26" s="133"/>
-      <c r="H26" s="167"/>
-      <c r="I26" s="168"/>
-      <c r="J26" s="169"/>
+      <c r="F26" s="137"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="178"/>
+      <c r="I26" s="179"/>
+      <c r="J26" s="180"/>
     </row>
     <row r="27" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
@@ -7666,11 +7994,11 @@
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="131"/>
-      <c r="G27" s="133"/>
-      <c r="H27" s="167"/>
-      <c r="I27" s="168"/>
-      <c r="J27" s="169"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="139"/>
+      <c r="H27" s="178"/>
+      <c r="I27" s="179"/>
+      <c r="J27" s="180"/>
     </row>
     <row r="28" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
@@ -7680,11 +8008,11 @@
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="131"/>
-      <c r="G28" s="133"/>
-      <c r="H28" s="167"/>
-      <c r="I28" s="168"/>
-      <c r="J28" s="169"/>
+      <c r="F28" s="137"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="178"/>
+      <c r="I28" s="179"/>
+      <c r="J28" s="180"/>
     </row>
     <row r="29" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33">
@@ -7694,11 +8022,11 @@
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
-      <c r="F29" s="131"/>
-      <c r="G29" s="133"/>
-      <c r="H29" s="167"/>
-      <c r="I29" s="168"/>
-      <c r="J29" s="169"/>
+      <c r="F29" s="137"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="178"/>
+      <c r="I29" s="179"/>
+      <c r="J29" s="180"/>
     </row>
     <row r="30" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A30" s="33">
@@ -7708,11 +8036,11 @@
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="131"/>
-      <c r="G30" s="133"/>
-      <c r="H30" s="167"/>
-      <c r="I30" s="168"/>
-      <c r="J30" s="169"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="178"/>
+      <c r="I30" s="179"/>
+      <c r="J30" s="180"/>
     </row>
     <row r="31" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A31" s="33">
@@ -7722,11 +8050,11 @@
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
-      <c r="F31" s="131"/>
-      <c r="G31" s="133"/>
-      <c r="H31" s="167"/>
-      <c r="I31" s="168"/>
-      <c r="J31" s="169"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="139"/>
+      <c r="H31" s="178"/>
+      <c r="I31" s="179"/>
+      <c r="J31" s="180"/>
     </row>
     <row r="32" spans="1:18" ht="11.25">
       <c r="A32" s="33">
@@ -7736,11 +8064,11 @@
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
-      <c r="F32" s="131"/>
-      <c r="G32" s="133"/>
-      <c r="H32" s="167"/>
-      <c r="I32" s="168"/>
-      <c r="J32" s="169"/>
+      <c r="F32" s="137"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="178"/>
+      <c r="I32" s="179"/>
+      <c r="J32" s="180"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
@@ -7757,11 +8085,11 @@
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="131"/>
-      <c r="G33" s="133"/>
-      <c r="H33" s="167"/>
-      <c r="I33" s="168"/>
-      <c r="J33" s="169"/>
+      <c r="F33" s="137"/>
+      <c r="G33" s="139"/>
+      <c r="H33" s="178"/>
+      <c r="I33" s="179"/>
+      <c r="J33" s="180"/>
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
@@ -7778,11 +8106,11 @@
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
-      <c r="F34" s="131"/>
-      <c r="G34" s="133"/>
-      <c r="H34" s="167"/>
-      <c r="I34" s="168"/>
-      <c r="J34" s="169"/>
+      <c r="F34" s="137"/>
+      <c r="G34" s="139"/>
+      <c r="H34" s="178"/>
+      <c r="I34" s="179"/>
+      <c r="J34" s="180"/>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
@@ -7799,11 +8127,11 @@
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
-      <c r="F35" s="131"/>
-      <c r="G35" s="133"/>
-      <c r="H35" s="167"/>
-      <c r="I35" s="168"/>
-      <c r="J35" s="169"/>
+      <c r="F35" s="137"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="178"/>
+      <c r="I35" s="179"/>
+      <c r="J35" s="180"/>
       <c r="L35" s="22"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
@@ -7820,11 +8148,11 @@
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="32"/>
-      <c r="F36" s="131"/>
-      <c r="G36" s="133"/>
-      <c r="H36" s="167"/>
-      <c r="I36" s="168"/>
-      <c r="J36" s="169"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="139"/>
+      <c r="H36" s="178"/>
+      <c r="I36" s="179"/>
+      <c r="J36" s="180"/>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
@@ -7841,11 +8169,11 @@
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
-      <c r="F37" s="131"/>
-      <c r="G37" s="133"/>
-      <c r="H37" s="167"/>
-      <c r="I37" s="168"/>
-      <c r="J37" s="169"/>
+      <c r="F37" s="137"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="178"/>
+      <c r="I37" s="179"/>
+      <c r="J37" s="180"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
@@ -7862,11 +8190,11 @@
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="32"/>
-      <c r="F38" s="131"/>
-      <c r="G38" s="133"/>
-      <c r="H38" s="167"/>
-      <c r="I38" s="168"/>
-      <c r="J38" s="169"/>
+      <c r="F38" s="137"/>
+      <c r="G38" s="139"/>
+      <c r="H38" s="178"/>
+      <c r="I38" s="179"/>
+      <c r="J38" s="180"/>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
@@ -7883,11 +8211,11 @@
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="131"/>
-      <c r="G39" s="133"/>
-      <c r="H39" s="167"/>
-      <c r="I39" s="168"/>
-      <c r="J39" s="169"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="139"/>
+      <c r="H39" s="178"/>
+      <c r="I39" s="179"/>
+      <c r="J39" s="180"/>
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
@@ -7904,11 +8232,11 @@
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="32"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="133"/>
-      <c r="H40" s="167"/>
-      <c r="I40" s="168"/>
-      <c r="J40" s="169"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="139"/>
+      <c r="H40" s="178"/>
+      <c r="I40" s="179"/>
+      <c r="J40" s="180"/>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
@@ -7925,11 +8253,11 @@
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
-      <c r="F41" s="131"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="167"/>
-      <c r="I41" s="168"/>
-      <c r="J41" s="169"/>
+      <c r="F41" s="137"/>
+      <c r="G41" s="139"/>
+      <c r="H41" s="178"/>
+      <c r="I41" s="179"/>
+      <c r="J41" s="180"/>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
@@ -7946,11 +8274,11 @@
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="32"/>
-      <c r="F42" s="131"/>
-      <c r="G42" s="133"/>
-      <c r="H42" s="167"/>
-      <c r="I42" s="168"/>
-      <c r="J42" s="169"/>
+      <c r="F42" s="137"/>
+      <c r="G42" s="139"/>
+      <c r="H42" s="178"/>
+      <c r="I42" s="179"/>
+      <c r="J42" s="180"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
@@ -7967,11 +8295,11 @@
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="32"/>
-      <c r="F43" s="131"/>
-      <c r="G43" s="133"/>
-      <c r="H43" s="167"/>
-      <c r="I43" s="168"/>
-      <c r="J43" s="169"/>
+      <c r="F43" s="137"/>
+      <c r="G43" s="139"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="179"/>
+      <c r="J43" s="180"/>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
@@ -7988,11 +8316,11 @@
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
       <c r="E44" s="32"/>
-      <c r="F44" s="131"/>
-      <c r="G44" s="133"/>
-      <c r="H44" s="167"/>
-      <c r="I44" s="168"/>
-      <c r="J44" s="169"/>
+      <c r="F44" s="137"/>
+      <c r="G44" s="139"/>
+      <c r="H44" s="178"/>
+      <c r="I44" s="179"/>
+      <c r="J44" s="180"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
@@ -8009,11 +8337,11 @@
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
       <c r="E45" s="32"/>
-      <c r="F45" s="131"/>
-      <c r="G45" s="133"/>
-      <c r="H45" s="167"/>
-      <c r="I45" s="168"/>
-      <c r="J45" s="169"/>
+      <c r="F45" s="137"/>
+      <c r="G45" s="139"/>
+      <c r="H45" s="178"/>
+      <c r="I45" s="179"/>
+      <c r="J45" s="180"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
@@ -8030,11 +8358,11 @@
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
       <c r="E46" s="32"/>
-      <c r="F46" s="131"/>
-      <c r="G46" s="133"/>
-      <c r="H46" s="167"/>
-      <c r="I46" s="168"/>
-      <c r="J46" s="169"/>
+      <c r="F46" s="137"/>
+      <c r="G46" s="139"/>
+      <c r="H46" s="178"/>
+      <c r="I46" s="179"/>
+      <c r="J46" s="180"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
@@ -8051,11 +8379,11 @@
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="32"/>
-      <c r="F47" s="131"/>
-      <c r="G47" s="133"/>
-      <c r="H47" s="167"/>
-      <c r="I47" s="168"/>
-      <c r="J47" s="169"/>
+      <c r="F47" s="137"/>
+      <c r="G47" s="139"/>
+      <c r="H47" s="178"/>
+      <c r="I47" s="179"/>
+      <c r="J47" s="180"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
@@ -8072,11 +8400,11 @@
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="32"/>
-      <c r="F48" s="131"/>
-      <c r="G48" s="133"/>
-      <c r="H48" s="167"/>
-      <c r="I48" s="168"/>
-      <c r="J48" s="169"/>
+      <c r="F48" s="137"/>
+      <c r="G48" s="139"/>
+      <c r="H48" s="178"/>
+      <c r="I48" s="179"/>
+      <c r="J48" s="180"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
@@ -8093,11 +8421,11 @@
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
-      <c r="F49" s="131"/>
-      <c r="G49" s="133"/>
-      <c r="H49" s="167"/>
-      <c r="I49" s="168"/>
-      <c r="J49" s="169"/>
+      <c r="F49" s="137"/>
+      <c r="G49" s="139"/>
+      <c r="H49" s="178"/>
+      <c r="I49" s="179"/>
+      <c r="J49" s="180"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
@@ -8114,11 +8442,11 @@
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="32"/>
-      <c r="F50" s="131"/>
-      <c r="G50" s="133"/>
-      <c r="H50" s="167"/>
-      <c r="I50" s="168"/>
-      <c r="J50" s="169"/>
+      <c r="F50" s="137"/>
+      <c r="G50" s="139"/>
+      <c r="H50" s="178"/>
+      <c r="I50" s="179"/>
+      <c r="J50" s="180"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
@@ -8135,11 +8463,11 @@
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="32"/>
-      <c r="F51" s="131"/>
-      <c r="G51" s="133"/>
-      <c r="H51" s="167"/>
-      <c r="I51" s="168"/>
-      <c r="J51" s="169"/>
+      <c r="F51" s="137"/>
+      <c r="G51" s="139"/>
+      <c r="H51" s="178"/>
+      <c r="I51" s="179"/>
+      <c r="J51" s="180"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
@@ -8156,11 +8484,11 @@
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="32"/>
-      <c r="F52" s="131"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="167"/>
-      <c r="I52" s="168"/>
-      <c r="J52" s="169"/>
+      <c r="F52" s="137"/>
+      <c r="G52" s="139"/>
+      <c r="H52" s="178"/>
+      <c r="I52" s="179"/>
+      <c r="J52" s="180"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
@@ -8177,11 +8505,11 @@
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="131"/>
-      <c r="G53" s="133"/>
-      <c r="H53" s="167"/>
-      <c r="I53" s="168"/>
-      <c r="J53" s="169"/>
+      <c r="F53" s="137"/>
+      <c r="G53" s="139"/>
+      <c r="H53" s="178"/>
+      <c r="I53" s="179"/>
+      <c r="J53" s="180"/>
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
@@ -8198,11 +8526,11 @@
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="32"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="133"/>
-      <c r="H54" s="167"/>
-      <c r="I54" s="168"/>
-      <c r="J54" s="169"/>
+      <c r="F54" s="137"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="178"/>
+      <c r="I54" s="179"/>
+      <c r="J54" s="180"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
@@ -8219,11 +8547,11 @@
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="32"/>
-      <c r="F55" s="131"/>
-      <c r="G55" s="133"/>
-      <c r="H55" s="167"/>
-      <c r="I55" s="168"/>
-      <c r="J55" s="169"/>
+      <c r="F55" s="137"/>
+      <c r="G55" s="139"/>
+      <c r="H55" s="178"/>
+      <c r="I55" s="179"/>
+      <c r="J55" s="180"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
@@ -8240,11 +8568,11 @@
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
       <c r="E56" s="32"/>
-      <c r="F56" s="131"/>
-      <c r="G56" s="133"/>
-      <c r="H56" s="167"/>
-      <c r="I56" s="168"/>
-      <c r="J56" s="169"/>
+      <c r="F56" s="137"/>
+      <c r="G56" s="139"/>
+      <c r="H56" s="178"/>
+      <c r="I56" s="179"/>
+      <c r="J56" s="180"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
@@ -8364,7 +8692,7 @@
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="F11:G11"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E56">
       <formula1>"Text,Number,Boolean,Datatime,Object,Structure"</formula1>
     </dataValidation>
@@ -8381,7 +8709,7 @@
   <dimension ref="A1:Q1048467"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -8404,20 +8732,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
       <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="173" t="str">
+      <c r="F1" s="187" t="str">
         <f>'Update History'!D1</f>
         <v>ASOFT - ERP.NET</v>
       </c>
-      <c r="G1" s="173"/>
+      <c r="G1" s="187"/>
       <c r="H1" s="26" t="s">
         <v>3</v>
       </c>
@@ -8445,18 +8773,18 @@
       <c r="Q1" s="52"/>
     </row>
     <row r="2" spans="1:17" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
       <c r="E2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="173" t="str">
+      <c r="F2" s="187" t="str">
         <f>'Update History'!D2</f>
         <v>ASOFT - CI</v>
       </c>
-      <c r="G2" s="173"/>
+      <c r="G2" s="187"/>
       <c r="H2" s="26" t="s">
         <v>49</v>
       </c>
@@ -8502,12 +8830,12 @@
       <c r="F4" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="143" t="s">
+      <c r="G4" s="149" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145"/>
-      <c r="J4" s="144"/>
+      <c r="H4" s="151"/>
+      <c r="I4" s="151"/>
+      <c r="J4" s="150"/>
       <c r="K4" s="39" t="s">
         <v>56</v>
       </c>
@@ -8543,12 +8871,12 @@
       <c r="F5" s="126" t="s">
         <v>196</v>
       </c>
-      <c r="G5" s="134" t="s">
+      <c r="G5" s="184" t="s">
         <v>218</v>
       </c>
-      <c r="H5" s="135"/>
-      <c r="I5" s="135"/>
-      <c r="J5" s="136"/>
+      <c r="H5" s="185"/>
+      <c r="I5" s="185"/>
+      <c r="J5" s="186"/>
       <c r="K5" s="116"/>
       <c r="L5" s="117"/>
       <c r="M5" s="74" t="s">
@@ -8582,12 +8910,12 @@
       <c r="F6" s="126" t="s">
         <v>190</v>
       </c>
-      <c r="G6" s="134" t="s">
+      <c r="G6" s="140" t="s">
         <v>191</v>
       </c>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="136"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="142"/>
       <c r="K6" s="117" t="s">
         <v>192</v>
       </c>
@@ -8625,12 +8953,12 @@
       <c r="F7" s="126" t="s">
         <v>199</v>
       </c>
-      <c r="G7" s="134" t="s">
+      <c r="G7" s="184" t="s">
         <v>211</v>
       </c>
-      <c r="H7" s="135"/>
-      <c r="I7" s="135"/>
-      <c r="J7" s="136"/>
+      <c r="H7" s="185"/>
+      <c r="I7" s="185"/>
+      <c r="J7" s="186"/>
       <c r="K7" s="87"/>
       <c r="L7" s="87"/>
       <c r="M7" s="74" t="s">
@@ -8664,12 +8992,12 @@
       <c r="F8" s="126" t="s">
         <v>202</v>
       </c>
-      <c r="G8" s="134" t="s">
+      <c r="G8" s="184" t="s">
         <v>219</v>
       </c>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="136"/>
+      <c r="H8" s="185"/>
+      <c r="I8" s="185"/>
+      <c r="J8" s="186"/>
       <c r="K8" s="129" t="s">
         <v>221</v>
       </c>
@@ -8697,10 +9025,10 @@
       <c r="D9" s="63"/>
       <c r="E9" s="63"/>
       <c r="F9" s="80"/>
-      <c r="G9" s="170"/>
-      <c r="H9" s="171"/>
-      <c r="I9" s="171"/>
-      <c r="J9" s="172"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="182"/>
+      <c r="I9" s="182"/>
+      <c r="J9" s="183"/>
       <c r="K9" s="87"/>
       <c r="L9" s="87"/>
       <c r="M9" s="74"/>
@@ -8718,10 +9046,10 @@
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
       <c r="F10" s="80"/>
-      <c r="G10" s="170"/>
-      <c r="H10" s="171"/>
-      <c r="I10" s="171"/>
-      <c r="J10" s="172"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="182"/>
+      <c r="J10" s="183"/>
       <c r="K10" s="87"/>
       <c r="L10" s="87"/>
       <c r="M10" s="74"/>
@@ -8739,10 +9067,10 @@
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
       <c r="F11" s="80"/>
-      <c r="G11" s="170"/>
-      <c r="H11" s="171"/>
-      <c r="I11" s="171"/>
-      <c r="J11" s="172"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="182"/>
+      <c r="I11" s="182"/>
+      <c r="J11" s="183"/>
       <c r="K11" s="87"/>
       <c r="L11" s="87"/>
       <c r="M11" s="74"/>
@@ -8760,10 +9088,10 @@
       <c r="D12" s="63"/>
       <c r="E12" s="63"/>
       <c r="F12" s="80"/>
-      <c r="G12" s="170"/>
-      <c r="H12" s="171"/>
-      <c r="I12" s="171"/>
-      <c r="J12" s="172"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="182"/>
+      <c r="I12" s="182"/>
+      <c r="J12" s="183"/>
       <c r="K12" s="83"/>
       <c r="L12" s="83"/>
       <c r="M12" s="74"/>
@@ -8781,10 +9109,10 @@
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
       <c r="F13" s="80"/>
-      <c r="G13" s="170"/>
-      <c r="H13" s="171"/>
-      <c r="I13" s="171"/>
-      <c r="J13" s="172"/>
+      <c r="G13" s="181"/>
+      <c r="H13" s="182"/>
+      <c r="I13" s="182"/>
+      <c r="J13" s="183"/>
       <c r="K13" s="83"/>
       <c r="L13" s="83"/>
       <c r="M13" s="74"/>
@@ -8802,10 +9130,10 @@
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
       <c r="F14" s="80"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="171"/>
-      <c r="I14" s="171"/>
-      <c r="J14" s="172"/>
+      <c r="G14" s="181"/>
+      <c r="H14" s="182"/>
+      <c r="I14" s="182"/>
+      <c r="J14" s="183"/>
       <c r="K14" s="79"/>
       <c r="L14" s="79"/>
       <c r="M14" s="74"/>
@@ -8823,10 +9151,10 @@
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
       <c r="F15" s="80"/>
-      <c r="G15" s="170"/>
-      <c r="H15" s="171"/>
-      <c r="I15" s="171"/>
-      <c r="J15" s="172"/>
+      <c r="G15" s="181"/>
+      <c r="H15" s="182"/>
+      <c r="I15" s="182"/>
+      <c r="J15" s="183"/>
       <c r="K15" s="79"/>
       <c r="L15" s="79"/>
       <c r="M15" s="74"/>
@@ -8844,10 +9172,10 @@
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
       <c r="F16" s="40"/>
-      <c r="G16" s="170"/>
-      <c r="H16" s="171"/>
-      <c r="I16" s="171"/>
-      <c r="J16" s="172"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="182"/>
+      <c r="I16" s="182"/>
+      <c r="J16" s="183"/>
       <c r="K16" s="71"/>
       <c r="L16" s="60"/>
       <c r="M16" s="74"/>
@@ -8865,10 +9193,10 @@
       <c r="D17" s="63"/>
       <c r="E17" s="63"/>
       <c r="F17" s="40"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="171"/>
-      <c r="I17" s="171"/>
-      <c r="J17" s="172"/>
+      <c r="G17" s="181"/>
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="183"/>
       <c r="K17" s="60"/>
       <c r="L17" s="60"/>
       <c r="M17" s="74"/>
@@ -8886,10 +9214,10 @@
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
       <c r="F18" s="40"/>
-      <c r="G18" s="170"/>
-      <c r="H18" s="171"/>
-      <c r="I18" s="171"/>
-      <c r="J18" s="172"/>
+      <c r="G18" s="181"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="182"/>
+      <c r="J18" s="183"/>
       <c r="K18" s="60"/>
       <c r="L18" s="60"/>
       <c r="M18" s="74"/>
@@ -8907,10 +9235,10 @@
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
       <c r="F19" s="40"/>
-      <c r="G19" s="170"/>
-      <c r="H19" s="171"/>
-      <c r="I19" s="171"/>
-      <c r="J19" s="172"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="182"/>
+      <c r="I19" s="182"/>
+      <c r="J19" s="183"/>
       <c r="K19" s="60"/>
       <c r="L19" s="60"/>
       <c r="M19" s="74"/>
@@ -8928,10 +9256,10 @@
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
       <c r="F20" s="40"/>
-      <c r="G20" s="170"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="171"/>
-      <c r="J20" s="172"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="183"/>
       <c r="K20" s="60"/>
       <c r="L20" s="60"/>
       <c r="M20" s="74"/>
@@ -8949,10 +9277,10 @@
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
       <c r="F21" s="40"/>
-      <c r="G21" s="170"/>
-      <c r="H21" s="171"/>
-      <c r="I21" s="171"/>
-      <c r="J21" s="172"/>
+      <c r="G21" s="181"/>
+      <c r="H21" s="182"/>
+      <c r="I21" s="182"/>
+      <c r="J21" s="183"/>
       <c r="K21" s="60"/>
       <c r="L21" s="60"/>
       <c r="M21" s="74"/>
@@ -8970,10 +9298,10 @@
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
       <c r="F22" s="40"/>
-      <c r="G22" s="170"/>
-      <c r="H22" s="171"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="172"/>
+      <c r="G22" s="181"/>
+      <c r="H22" s="182"/>
+      <c r="I22" s="182"/>
+      <c r="J22" s="183"/>
       <c r="K22" s="60"/>
       <c r="L22" s="60"/>
       <c r="M22" s="74"/>
@@ -8991,10 +9319,10 @@
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
       <c r="F23" s="40"/>
-      <c r="G23" s="170"/>
-      <c r="H23" s="171"/>
-      <c r="I23" s="171"/>
-      <c r="J23" s="172"/>
+      <c r="G23" s="181"/>
+      <c r="H23" s="182"/>
+      <c r="I23" s="182"/>
+      <c r="J23" s="183"/>
       <c r="K23" s="60"/>
       <c r="L23" s="60"/>
       <c r="M23" s="74"/>
@@ -9012,10 +9340,10 @@
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
       <c r="F24" s="40"/>
-      <c r="G24" s="170"/>
-      <c r="H24" s="171"/>
-      <c r="I24" s="171"/>
-      <c r="J24" s="172"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="182"/>
+      <c r="I24" s="182"/>
+      <c r="J24" s="183"/>
       <c r="K24" s="60"/>
       <c r="L24" s="60"/>
       <c r="M24" s="74"/>
@@ -9033,10 +9361,10 @@
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
       <c r="F25" s="40"/>
-      <c r="G25" s="170"/>
-      <c r="H25" s="171"/>
-      <c r="I25" s="171"/>
-      <c r="J25" s="172"/>
+      <c r="G25" s="181"/>
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="183"/>
       <c r="K25" s="60"/>
       <c r="L25" s="60"/>
       <c r="M25" s="74"/>
@@ -9054,10 +9382,10 @@
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
       <c r="F26" s="40"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="171"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="172"/>
+      <c r="G26" s="181"/>
+      <c r="H26" s="182"/>
+      <c r="I26" s="182"/>
+      <c r="J26" s="183"/>
       <c r="K26" s="60"/>
       <c r="L26" s="60"/>
       <c r="M26" s="74"/>
@@ -9075,10 +9403,10 @@
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
       <c r="F27" s="40"/>
-      <c r="G27" s="170"/>
-      <c r="H27" s="171"/>
-      <c r="I27" s="171"/>
-      <c r="J27" s="172"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="182"/>
+      <c r="I27" s="182"/>
+      <c r="J27" s="183"/>
       <c r="K27" s="60"/>
       <c r="L27" s="60"/>
       <c r="M27" s="74"/>
@@ -9096,10 +9424,10 @@
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
       <c r="F28" s="40"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="171"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="172"/>
+      <c r="G28" s="181"/>
+      <c r="H28" s="182"/>
+      <c r="I28" s="182"/>
+      <c r="J28" s="183"/>
       <c r="K28" s="60"/>
       <c r="L28" s="60"/>
       <c r="M28" s="74"/>
@@ -9117,10 +9445,10 @@
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
       <c r="F29" s="40"/>
-      <c r="G29" s="170"/>
-      <c r="H29" s="171"/>
-      <c r="I29" s="171"/>
-      <c r="J29" s="172"/>
+      <c r="G29" s="181"/>
+      <c r="H29" s="182"/>
+      <c r="I29" s="182"/>
+      <c r="J29" s="183"/>
       <c r="K29" s="60"/>
       <c r="L29" s="60"/>
       <c r="M29" s="74"/>
@@ -9138,10 +9466,10 @@
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
       <c r="F30" s="40"/>
-      <c r="G30" s="170"/>
-      <c r="H30" s="171"/>
-      <c r="I30" s="171"/>
-      <c r="J30" s="172"/>
+      <c r="G30" s="181"/>
+      <c r="H30" s="182"/>
+      <c r="I30" s="182"/>
+      <c r="J30" s="183"/>
       <c r="K30" s="60"/>
       <c r="L30" s="60"/>
       <c r="M30" s="74"/>
@@ -9159,10 +9487,10 @@
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
       <c r="F31" s="40"/>
-      <c r="G31" s="170"/>
-      <c r="H31" s="171"/>
-      <c r="I31" s="171"/>
-      <c r="J31" s="172"/>
+      <c r="G31" s="181"/>
+      <c r="H31" s="182"/>
+      <c r="I31" s="182"/>
+      <c r="J31" s="183"/>
       <c r="K31" s="60"/>
       <c r="L31" s="60"/>
       <c r="M31" s="74"/>
@@ -9180,10 +9508,10 @@
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
       <c r="F32" s="40"/>
-      <c r="G32" s="170"/>
-      <c r="H32" s="171"/>
-      <c r="I32" s="171"/>
-      <c r="J32" s="172"/>
+      <c r="G32" s="181"/>
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="183"/>
       <c r="K32" s="60"/>
       <c r="L32" s="60"/>
       <c r="M32" s="74"/>
@@ -9201,10 +9529,10 @@
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
       <c r="F33" s="40"/>
-      <c r="G33" s="170"/>
-      <c r="H33" s="171"/>
-      <c r="I33" s="171"/>
-      <c r="J33" s="172"/>
+      <c r="G33" s="181"/>
+      <c r="H33" s="182"/>
+      <c r="I33" s="182"/>
+      <c r="J33" s="183"/>
       <c r="K33" s="60"/>
       <c r="L33" s="60"/>
       <c r="M33" s="74"/>
@@ -9222,10 +9550,10 @@
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
       <c r="F34" s="80"/>
-      <c r="G34" s="170"/>
-      <c r="H34" s="171"/>
-      <c r="I34" s="171"/>
-      <c r="J34" s="172"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="182"/>
+      <c r="I34" s="182"/>
+      <c r="J34" s="183"/>
       <c r="K34" s="83"/>
       <c r="L34" s="83"/>
       <c r="M34" s="74"/>
@@ -9243,10 +9571,10 @@
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
       <c r="F35" s="40"/>
-      <c r="G35" s="170"/>
-      <c r="H35" s="171"/>
-      <c r="I35" s="171"/>
-      <c r="J35" s="172"/>
+      <c r="G35" s="181"/>
+      <c r="H35" s="182"/>
+      <c r="I35" s="182"/>
+      <c r="J35" s="183"/>
       <c r="K35" s="60"/>
       <c r="L35" s="60"/>
       <c r="M35" s="74"/>
@@ -9264,10 +9592,10 @@
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
       <c r="F36" s="40"/>
-      <c r="G36" s="170"/>
-      <c r="H36" s="171"/>
-      <c r="I36" s="171"/>
-      <c r="J36" s="172"/>
+      <c r="G36" s="181"/>
+      <c r="H36" s="182"/>
+      <c r="I36" s="182"/>
+      <c r="J36" s="183"/>
       <c r="K36" s="60"/>
       <c r="L36" s="60"/>
       <c r="M36" s="74"/>
@@ -9285,10 +9613,10 @@
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
       <c r="F37" s="40"/>
-      <c r="G37" s="170"/>
-      <c r="H37" s="171"/>
-      <c r="I37" s="171"/>
-      <c r="J37" s="172"/>
+      <c r="G37" s="181"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="183"/>
       <c r="K37" s="60"/>
       <c r="L37" s="60"/>
       <c r="M37" s="74"/>
@@ -9306,10 +9634,10 @@
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
       <c r="F38" s="40"/>
-      <c r="G38" s="170"/>
-      <c r="H38" s="171"/>
-      <c r="I38" s="171"/>
-      <c r="J38" s="172"/>
+      <c r="G38" s="181"/>
+      <c r="H38" s="182"/>
+      <c r="I38" s="182"/>
+      <c r="J38" s="183"/>
       <c r="K38" s="60"/>
       <c r="L38" s="60"/>
       <c r="M38" s="74"/>
@@ -9327,10 +9655,10 @@
       <c r="D39" s="63"/>
       <c r="E39" s="63"/>
       <c r="F39" s="40"/>
-      <c r="G39" s="170"/>
-      <c r="H39" s="171"/>
-      <c r="I39" s="171"/>
-      <c r="J39" s="172"/>
+      <c r="G39" s="181"/>
+      <c r="H39" s="182"/>
+      <c r="I39" s="182"/>
+      <c r="J39" s="183"/>
       <c r="K39" s="60"/>
       <c r="L39" s="60"/>
       <c r="M39" s="74"/>
@@ -9348,10 +9676,10 @@
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
       <c r="F40" s="40"/>
-      <c r="G40" s="170"/>
-      <c r="H40" s="171"/>
-      <c r="I40" s="171"/>
-      <c r="J40" s="172"/>
+      <c r="G40" s="181"/>
+      <c r="H40" s="182"/>
+      <c r="I40" s="182"/>
+      <c r="J40" s="183"/>
       <c r="K40" s="73"/>
       <c r="L40" s="73"/>
       <c r="M40" s="74"/>
@@ -9369,10 +9697,10 @@
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
       <c r="F41" s="40"/>
-      <c r="G41" s="170"/>
-      <c r="H41" s="171"/>
-      <c r="I41" s="171"/>
-      <c r="J41" s="172"/>
+      <c r="G41" s="181"/>
+      <c r="H41" s="182"/>
+      <c r="I41" s="182"/>
+      <c r="J41" s="183"/>
       <c r="K41" s="73"/>
       <c r="L41" s="73"/>
       <c r="M41" s="74"/>
@@ -9390,10 +9718,10 @@
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
       <c r="F42" s="40"/>
-      <c r="G42" s="170"/>
-      <c r="H42" s="171"/>
-      <c r="I42" s="171"/>
-      <c r="J42" s="172"/>
+      <c r="G42" s="181"/>
+      <c r="H42" s="182"/>
+      <c r="I42" s="182"/>
+      <c r="J42" s="183"/>
       <c r="K42" s="73"/>
       <c r="L42" s="73"/>
       <c r="M42" s="74"/>
@@ -9411,10 +9739,10 @@
       <c r="D43" s="63"/>
       <c r="E43" s="63"/>
       <c r="F43" s="40"/>
-      <c r="G43" s="170"/>
-      <c r="H43" s="171"/>
-      <c r="I43" s="171"/>
-      <c r="J43" s="172"/>
+      <c r="G43" s="181"/>
+      <c r="H43" s="182"/>
+      <c r="I43" s="182"/>
+      <c r="J43" s="183"/>
       <c r="K43" s="73"/>
       <c r="L43" s="73"/>
       <c r="M43" s="74"/>
@@ -9432,10 +9760,10 @@
       <c r="D44" s="63"/>
       <c r="E44" s="63"/>
       <c r="F44" s="40"/>
-      <c r="G44" s="170"/>
-      <c r="H44" s="171"/>
-      <c r="I44" s="171"/>
-      <c r="J44" s="172"/>
+      <c r="G44" s="181"/>
+      <c r="H44" s="182"/>
+      <c r="I44" s="182"/>
+      <c r="J44" s="183"/>
       <c r="K44" s="73"/>
       <c r="L44" s="73"/>
       <c r="M44" s="74"/>
@@ -9453,10 +9781,10 @@
       <c r="D45" s="63"/>
       <c r="E45" s="63"/>
       <c r="F45" s="40"/>
-      <c r="G45" s="170"/>
-      <c r="H45" s="171"/>
-      <c r="I45" s="171"/>
-      <c r="J45" s="172"/>
+      <c r="G45" s="181"/>
+      <c r="H45" s="182"/>
+      <c r="I45" s="182"/>
+      <c r="J45" s="183"/>
       <c r="K45" s="73"/>
       <c r="L45" s="73"/>
       <c r="M45" s="74"/>
@@ -9474,10 +9802,10 @@
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
       <c r="F46" s="40"/>
-      <c r="G46" s="170"/>
-      <c r="H46" s="171"/>
-      <c r="I46" s="171"/>
-      <c r="J46" s="172"/>
+      <c r="G46" s="181"/>
+      <c r="H46" s="182"/>
+      <c r="I46" s="182"/>
+      <c r="J46" s="183"/>
       <c r="K46" s="73"/>
       <c r="L46" s="73"/>
       <c r="M46" s="74"/>
@@ -9495,10 +9823,10 @@
       <c r="D47" s="63"/>
       <c r="E47" s="63"/>
       <c r="F47" s="40"/>
-      <c r="G47" s="170"/>
-      <c r="H47" s="171"/>
-      <c r="I47" s="171"/>
-      <c r="J47" s="172"/>
+      <c r="G47" s="181"/>
+      <c r="H47" s="182"/>
+      <c r="I47" s="182"/>
+      <c r="J47" s="183"/>
       <c r="K47" s="73"/>
       <c r="L47" s="73"/>
       <c r="M47" s="74"/>
@@ -9516,10 +9844,10 @@
       <c r="D48" s="63"/>
       <c r="E48" s="63"/>
       <c r="F48" s="40"/>
-      <c r="G48" s="170"/>
-      <c r="H48" s="171"/>
-      <c r="I48" s="171"/>
-      <c r="J48" s="172"/>
+      <c r="G48" s="181"/>
+      <c r="H48" s="182"/>
+      <c r="I48" s="182"/>
+      <c r="J48" s="183"/>
       <c r="K48" s="73"/>
       <c r="L48" s="73"/>
       <c r="M48" s="74"/>
@@ -9537,10 +9865,10 @@
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
       <c r="F49" s="40"/>
-      <c r="G49" s="170"/>
-      <c r="H49" s="171"/>
-      <c r="I49" s="171"/>
-      <c r="J49" s="172"/>
+      <c r="G49" s="181"/>
+      <c r="H49" s="182"/>
+      <c r="I49" s="182"/>
+      <c r="J49" s="183"/>
       <c r="K49" s="73"/>
       <c r="L49" s="73"/>
       <c r="M49" s="74"/>
@@ -9558,10 +9886,10 @@
       <c r="D50" s="63"/>
       <c r="E50" s="63"/>
       <c r="F50" s="40"/>
-      <c r="G50" s="170"/>
-      <c r="H50" s="171"/>
-      <c r="I50" s="171"/>
-      <c r="J50" s="172"/>
+      <c r="G50" s="181"/>
+      <c r="H50" s="182"/>
+      <c r="I50" s="182"/>
+      <c r="J50" s="183"/>
       <c r="K50" s="73"/>
       <c r="L50" s="73"/>
       <c r="M50" s="74"/>
@@ -9579,10 +9907,10 @@
       <c r="D51" s="63"/>
       <c r="E51" s="63"/>
       <c r="F51" s="40"/>
-      <c r="G51" s="170"/>
-      <c r="H51" s="171"/>
-      <c r="I51" s="171"/>
-      <c r="J51" s="172"/>
+      <c r="G51" s="181"/>
+      <c r="H51" s="182"/>
+      <c r="I51" s="182"/>
+      <c r="J51" s="183"/>
       <c r="K51" s="73"/>
       <c r="L51" s="73"/>
       <c r="M51" s="74"/>
@@ -9600,10 +9928,10 @@
       <c r="D52" s="63"/>
       <c r="E52" s="63"/>
       <c r="F52" s="40"/>
-      <c r="G52" s="170"/>
-      <c r="H52" s="171"/>
-      <c r="I52" s="171"/>
-      <c r="J52" s="172"/>
+      <c r="G52" s="181"/>
+      <c r="H52" s="182"/>
+      <c r="I52" s="182"/>
+      <c r="J52" s="183"/>
       <c r="K52" s="73"/>
       <c r="L52" s="73"/>
       <c r="M52" s="74"/>
@@ -9621,10 +9949,10 @@
       <c r="D53" s="63"/>
       <c r="E53" s="63"/>
       <c r="F53" s="40"/>
-      <c r="G53" s="170"/>
-      <c r="H53" s="171"/>
-      <c r="I53" s="171"/>
-      <c r="J53" s="172"/>
+      <c r="G53" s="181"/>
+      <c r="H53" s="182"/>
+      <c r="I53" s="182"/>
+      <c r="J53" s="183"/>
       <c r="K53" s="73"/>
       <c r="L53" s="73"/>
       <c r="M53" s="74"/>
@@ -9642,10 +9970,10 @@
       <c r="D54" s="63"/>
       <c r="E54" s="63"/>
       <c r="F54" s="40"/>
-      <c r="G54" s="170"/>
-      <c r="H54" s="171"/>
-      <c r="I54" s="171"/>
-      <c r="J54" s="172"/>
+      <c r="G54" s="181"/>
+      <c r="H54" s="182"/>
+      <c r="I54" s="182"/>
+      <c r="J54" s="183"/>
       <c r="K54" s="73"/>
       <c r="L54" s="73"/>
       <c r="M54" s="74"/>
@@ -9663,10 +9991,10 @@
       <c r="D55" s="63"/>
       <c r="E55" s="63"/>
       <c r="F55" s="40"/>
-      <c r="G55" s="170"/>
-      <c r="H55" s="171"/>
-      <c r="I55" s="171"/>
-      <c r="J55" s="172"/>
+      <c r="G55" s="181"/>
+      <c r="H55" s="182"/>
+      <c r="I55" s="182"/>
+      <c r="J55" s="183"/>
       <c r="K55" s="73"/>
       <c r="L55" s="73"/>
       <c r="M55" s="74"/>
@@ -9684,10 +10012,10 @@
       <c r="D56" s="63"/>
       <c r="E56" s="63"/>
       <c r="F56" s="40"/>
-      <c r="G56" s="170"/>
-      <c r="H56" s="171"/>
-      <c r="I56" s="171"/>
-      <c r="J56" s="172"/>
+      <c r="G56" s="181"/>
+      <c r="H56" s="182"/>
+      <c r="I56" s="182"/>
+      <c r="J56" s="183"/>
       <c r="K56" s="73"/>
       <c r="L56" s="73"/>
       <c r="M56" s="74"/>
@@ -9705,10 +10033,10 @@
       <c r="D57" s="63"/>
       <c r="E57" s="63"/>
       <c r="F57" s="40"/>
-      <c r="G57" s="170"/>
-      <c r="H57" s="171"/>
-      <c r="I57" s="171"/>
-      <c r="J57" s="172"/>
+      <c r="G57" s="181"/>
+      <c r="H57" s="182"/>
+      <c r="I57" s="182"/>
+      <c r="J57" s="183"/>
       <c r="K57" s="73"/>
       <c r="L57" s="73"/>
       <c r="M57" s="74"/>
@@ -9726,10 +10054,10 @@
       <c r="D58" s="63"/>
       <c r="E58" s="63"/>
       <c r="F58" s="40"/>
-      <c r="G58" s="170"/>
-      <c r="H58" s="171"/>
-      <c r="I58" s="171"/>
-      <c r="J58" s="172"/>
+      <c r="G58" s="181"/>
+      <c r="H58" s="182"/>
+      <c r="I58" s="182"/>
+      <c r="J58" s="183"/>
       <c r="K58" s="73"/>
       <c r="L58" s="73"/>
       <c r="M58" s="74"/>
@@ -9747,10 +10075,10 @@
       <c r="D59" s="63"/>
       <c r="E59" s="63"/>
       <c r="F59" s="40"/>
-      <c r="G59" s="170"/>
-      <c r="H59" s="171"/>
-      <c r="I59" s="171"/>
-      <c r="J59" s="172"/>
+      <c r="G59" s="181"/>
+      <c r="H59" s="182"/>
+      <c r="I59" s="182"/>
+      <c r="J59" s="183"/>
       <c r="K59" s="73"/>
       <c r="L59" s="73"/>
       <c r="M59" s="74"/>
@@ -9768,10 +10096,10 @@
       <c r="D60" s="63"/>
       <c r="E60" s="63"/>
       <c r="F60" s="40"/>
-      <c r="G60" s="170"/>
-      <c r="H60" s="171"/>
-      <c r="I60" s="171"/>
-      <c r="J60" s="172"/>
+      <c r="G60" s="181"/>
+      <c r="H60" s="182"/>
+      <c r="I60" s="182"/>
+      <c r="J60" s="183"/>
       <c r="K60" s="73"/>
       <c r="L60" s="73"/>
       <c r="M60" s="74"/>
@@ -9789,10 +10117,10 @@
       <c r="D61" s="63"/>
       <c r="E61" s="63"/>
       <c r="F61" s="40"/>
-      <c r="G61" s="170"/>
-      <c r="H61" s="171"/>
-      <c r="I61" s="171"/>
-      <c r="J61" s="172"/>
+      <c r="G61" s="181"/>
+      <c r="H61" s="182"/>
+      <c r="I61" s="182"/>
+      <c r="J61" s="183"/>
       <c r="K61" s="73"/>
       <c r="L61" s="73"/>
       <c r="M61" s="74"/>
@@ -9810,10 +10138,10 @@
       <c r="D62" s="63"/>
       <c r="E62" s="63"/>
       <c r="F62" s="40"/>
-      <c r="G62" s="170"/>
-      <c r="H62" s="171"/>
-      <c r="I62" s="171"/>
-      <c r="J62" s="172"/>
+      <c r="G62" s="181"/>
+      <c r="H62" s="182"/>
+      <c r="I62" s="182"/>
+      <c r="J62" s="183"/>
       <c r="K62" s="82"/>
       <c r="L62" s="82"/>
       <c r="M62" s="74"/>
@@ -9831,10 +10159,10 @@
       <c r="D63" s="63"/>
       <c r="E63" s="63"/>
       <c r="F63" s="40"/>
-      <c r="G63" s="170"/>
-      <c r="H63" s="171"/>
-      <c r="I63" s="171"/>
-      <c r="J63" s="172"/>
+      <c r="G63" s="181"/>
+      <c r="H63" s="182"/>
+      <c r="I63" s="182"/>
+      <c r="J63" s="183"/>
       <c r="K63" s="82"/>
       <c r="L63" s="82"/>
       <c r="M63" s="74"/>
@@ -9852,10 +10180,10 @@
       <c r="D64" s="63"/>
       <c r="E64" s="63"/>
       <c r="F64" s="40"/>
-      <c r="G64" s="170"/>
-      <c r="H64" s="171"/>
-      <c r="I64" s="171"/>
-      <c r="J64" s="172"/>
+      <c r="G64" s="181"/>
+      <c r="H64" s="182"/>
+      <c r="I64" s="182"/>
+      <c r="J64" s="183"/>
       <c r="K64" s="82"/>
       <c r="L64" s="82"/>
       <c r="M64" s="74"/>
@@ -9871,10 +10199,10 @@
       <c r="D65" s="63"/>
       <c r="E65" s="63"/>
       <c r="F65" s="40"/>
-      <c r="G65" s="170"/>
-      <c r="H65" s="171"/>
-      <c r="I65" s="171"/>
-      <c r="J65" s="172"/>
+      <c r="G65" s="181"/>
+      <c r="H65" s="182"/>
+      <c r="I65" s="182"/>
+      <c r="J65" s="183"/>
       <c r="K65" s="82"/>
       <c r="L65" s="82"/>
       <c r="M65" s="74"/>
@@ -9890,10 +10218,10 @@
       <c r="D66" s="63"/>
       <c r="E66" s="63"/>
       <c r="F66" s="40"/>
-      <c r="G66" s="170"/>
-      <c r="H66" s="171"/>
-      <c r="I66" s="171"/>
-      <c r="J66" s="172"/>
+      <c r="G66" s="181"/>
+      <c r="H66" s="182"/>
+      <c r="I66" s="182"/>
+      <c r="J66" s="183"/>
       <c r="K66" s="82"/>
       <c r="L66" s="82"/>
       <c r="M66" s="74"/>
@@ -9909,10 +10237,10 @@
       <c r="D67" s="63"/>
       <c r="E67" s="63"/>
       <c r="F67" s="40"/>
-      <c r="G67" s="170"/>
-      <c r="H67" s="171"/>
-      <c r="I67" s="171"/>
-      <c r="J67" s="172"/>
+      <c r="G67" s="181"/>
+      <c r="H67" s="182"/>
+      <c r="I67" s="182"/>
+      <c r="J67" s="183"/>
       <c r="K67" s="82"/>
       <c r="L67" s="82"/>
       <c r="M67" s="74"/>
@@ -9928,10 +10256,10 @@
       <c r="D68" s="63"/>
       <c r="E68" s="63"/>
       <c r="F68" s="40"/>
-      <c r="G68" s="170"/>
-      <c r="H68" s="171"/>
-      <c r="I68" s="171"/>
-      <c r="J68" s="172"/>
+      <c r="G68" s="181"/>
+      <c r="H68" s="182"/>
+      <c r="I68" s="182"/>
+      <c r="J68" s="183"/>
       <c r="K68" s="82"/>
       <c r="L68" s="82"/>
       <c r="M68" s="74"/>
@@ -9947,10 +10275,10 @@
       <c r="D69" s="63"/>
       <c r="E69" s="63"/>
       <c r="F69" s="40"/>
-      <c r="G69" s="170"/>
-      <c r="H69" s="171"/>
-      <c r="I69" s="171"/>
-      <c r="J69" s="172"/>
+      <c r="G69" s="181"/>
+      <c r="H69" s="182"/>
+      <c r="I69" s="182"/>
+      <c r="J69" s="183"/>
       <c r="K69" s="82"/>
       <c r="L69" s="82"/>
       <c r="M69" s="74"/>
@@ -9966,10 +10294,10 @@
       <c r="D70" s="63"/>
       <c r="E70" s="63"/>
       <c r="F70" s="40"/>
-      <c r="G70" s="170"/>
-      <c r="H70" s="171"/>
-      <c r="I70" s="171"/>
-      <c r="J70" s="172"/>
+      <c r="G70" s="181"/>
+      <c r="H70" s="182"/>
+      <c r="I70" s="182"/>
+      <c r="J70" s="183"/>
       <c r="K70" s="82"/>
       <c r="L70" s="82"/>
       <c r="M70" s="74"/>
@@ -9985,10 +10313,10 @@
       <c r="D71" s="63"/>
       <c r="E71" s="63"/>
       <c r="F71" s="40"/>
-      <c r="G71" s="170"/>
-      <c r="H71" s="171"/>
-      <c r="I71" s="171"/>
-      <c r="J71" s="172"/>
+      <c r="G71" s="181"/>
+      <c r="H71" s="182"/>
+      <c r="I71" s="182"/>
+      <c r="J71" s="183"/>
       <c r="K71" s="82"/>
       <c r="L71" s="82"/>
       <c r="M71" s="74"/>
@@ -10004,10 +10332,10 @@
       <c r="D72" s="63"/>
       <c r="E72" s="63"/>
       <c r="F72" s="40"/>
-      <c r="G72" s="170"/>
-      <c r="H72" s="171"/>
-      <c r="I72" s="171"/>
-      <c r="J72" s="172"/>
+      <c r="G72" s="181"/>
+      <c r="H72" s="182"/>
+      <c r="I72" s="182"/>
+      <c r="J72" s="183"/>
       <c r="K72" s="82"/>
       <c r="L72" s="82"/>
       <c r="M72" s="74"/>
@@ -10023,10 +10351,10 @@
       <c r="D73" s="63"/>
       <c r="E73" s="63"/>
       <c r="F73" s="40"/>
-      <c r="G73" s="170"/>
-      <c r="H73" s="171"/>
-      <c r="I73" s="171"/>
-      <c r="J73" s="172"/>
+      <c r="G73" s="181"/>
+      <c r="H73" s="182"/>
+      <c r="I73" s="182"/>
+      <c r="J73" s="183"/>
       <c r="K73" s="82"/>
       <c r="L73" s="82"/>
       <c r="M73" s="74"/>
@@ -10042,10 +10370,10 @@
       <c r="D74" s="63"/>
       <c r="E74" s="63"/>
       <c r="F74" s="40"/>
-      <c r="G74" s="170"/>
-      <c r="H74" s="171"/>
-      <c r="I74" s="171"/>
-      <c r="J74" s="172"/>
+      <c r="G74" s="181"/>
+      <c r="H74" s="182"/>
+      <c r="I74" s="182"/>
+      <c r="J74" s="183"/>
       <c r="K74" s="82"/>
       <c r="L74" s="82"/>
       <c r="M74" s="74"/>
@@ -10061,10 +10389,10 @@
       <c r="D75" s="63"/>
       <c r="E75" s="63"/>
       <c r="F75" s="40"/>
-      <c r="G75" s="170"/>
-      <c r="H75" s="171"/>
-      <c r="I75" s="171"/>
-      <c r="J75" s="172"/>
+      <c r="G75" s="181"/>
+      <c r="H75" s="182"/>
+      <c r="I75" s="182"/>
+      <c r="J75" s="183"/>
       <c r="K75" s="82"/>
       <c r="L75" s="82"/>
       <c r="M75" s="74"/>
@@ -10080,10 +10408,10 @@
       <c r="D76" s="63"/>
       <c r="E76" s="63"/>
       <c r="F76" s="40"/>
-      <c r="G76" s="170"/>
-      <c r="H76" s="171"/>
-      <c r="I76" s="171"/>
-      <c r="J76" s="172"/>
+      <c r="G76" s="181"/>
+      <c r="H76" s="182"/>
+      <c r="I76" s="182"/>
+      <c r="J76" s="183"/>
       <c r="K76" s="82"/>
       <c r="L76" s="82"/>
       <c r="M76" s="74"/>
@@ -10099,10 +10427,10 @@
       <c r="D77" s="63"/>
       <c r="E77" s="63"/>
       <c r="F77" s="40"/>
-      <c r="G77" s="170"/>
-      <c r="H77" s="171"/>
-      <c r="I77" s="171"/>
-      <c r="J77" s="172"/>
+      <c r="G77" s="181"/>
+      <c r="H77" s="182"/>
+      <c r="I77" s="182"/>
+      <c r="J77" s="183"/>
       <c r="K77" s="82"/>
       <c r="L77" s="82"/>
       <c r="M77" s="74"/>
@@ -10118,10 +10446,10 @@
       <c r="D78" s="63"/>
       <c r="E78" s="63"/>
       <c r="F78" s="40"/>
-      <c r="G78" s="170"/>
-      <c r="H78" s="171"/>
-      <c r="I78" s="171"/>
-      <c r="J78" s="172"/>
+      <c r="G78" s="181"/>
+      <c r="H78" s="182"/>
+      <c r="I78" s="182"/>
+      <c r="J78" s="183"/>
       <c r="K78" s="82"/>
       <c r="L78" s="82"/>
       <c r="M78" s="74"/>
@@ -10137,10 +10465,10 @@
       <c r="D79" s="63"/>
       <c r="E79" s="63"/>
       <c r="F79" s="40"/>
-      <c r="G79" s="170"/>
-      <c r="H79" s="171"/>
-      <c r="I79" s="171"/>
-      <c r="J79" s="172"/>
+      <c r="G79" s="181"/>
+      <c r="H79" s="182"/>
+      <c r="I79" s="182"/>
+      <c r="J79" s="183"/>
       <c r="K79" s="82"/>
       <c r="L79" s="82"/>
       <c r="M79" s="74"/>
@@ -10156,10 +10484,10 @@
       <c r="D80" s="63"/>
       <c r="E80" s="63"/>
       <c r="F80" s="40"/>
-      <c r="G80" s="170"/>
-      <c r="H80" s="171"/>
-      <c r="I80" s="171"/>
-      <c r="J80" s="172"/>
+      <c r="G80" s="181"/>
+      <c r="H80" s="182"/>
+      <c r="I80" s="182"/>
+      <c r="J80" s="183"/>
       <c r="K80" s="82"/>
       <c r="L80" s="82"/>
       <c r="M80" s="74"/>
@@ -10175,10 +10503,10 @@
       <c r="D81" s="63"/>
       <c r="E81" s="63"/>
       <c r="F81" s="40"/>
-      <c r="G81" s="170"/>
-      <c r="H81" s="171"/>
-      <c r="I81" s="171"/>
-      <c r="J81" s="172"/>
+      <c r="G81" s="181"/>
+      <c r="H81" s="182"/>
+      <c r="I81" s="182"/>
+      <c r="J81" s="183"/>
       <c r="K81" s="82"/>
       <c r="L81" s="82"/>
       <c r="M81" s="74"/>
@@ -10194,10 +10522,10 @@
       <c r="D82" s="63"/>
       <c r="E82" s="63"/>
       <c r="F82" s="40"/>
-      <c r="G82" s="170"/>
-      <c r="H82" s="171"/>
-      <c r="I82" s="171"/>
-      <c r="J82" s="172"/>
+      <c r="G82" s="181"/>
+      <c r="H82" s="182"/>
+      <c r="I82" s="182"/>
+      <c r="J82" s="183"/>
       <c r="K82" s="82"/>
       <c r="L82" s="82"/>
       <c r="M82" s="74"/>
@@ -10213,10 +10541,10 @@
       <c r="D83" s="63"/>
       <c r="E83" s="63"/>
       <c r="F83" s="40"/>
-      <c r="G83" s="170"/>
-      <c r="H83" s="171"/>
-      <c r="I83" s="171"/>
-      <c r="J83" s="172"/>
+      <c r="G83" s="181"/>
+      <c r="H83" s="182"/>
+      <c r="I83" s="182"/>
+      <c r="J83" s="183"/>
       <c r="K83" s="82"/>
       <c r="L83" s="82"/>
       <c r="M83" s="74"/>
@@ -10232,10 +10560,10 @@
       <c r="D84" s="63"/>
       <c r="E84" s="63"/>
       <c r="F84" s="40"/>
-      <c r="G84" s="170"/>
-      <c r="H84" s="171"/>
-      <c r="I84" s="171"/>
-      <c r="J84" s="172"/>
+      <c r="G84" s="181"/>
+      <c r="H84" s="182"/>
+      <c r="I84" s="182"/>
+      <c r="J84" s="183"/>
       <c r="K84" s="82"/>
       <c r="L84" s="82"/>
       <c r="M84" s="74"/>
@@ -10251,10 +10579,10 @@
       <c r="D85" s="63"/>
       <c r="E85" s="63"/>
       <c r="F85" s="40"/>
-      <c r="G85" s="170"/>
-      <c r="H85" s="171"/>
-      <c r="I85" s="171"/>
-      <c r="J85" s="172"/>
+      <c r="G85" s="181"/>
+      <c r="H85" s="182"/>
+      <c r="I85" s="182"/>
+      <c r="J85" s="183"/>
       <c r="K85" s="82"/>
       <c r="L85" s="82"/>
       <c r="M85" s="74"/>
@@ -10270,10 +10598,10 @@
       <c r="D86" s="63"/>
       <c r="E86" s="63"/>
       <c r="F86" s="40"/>
-      <c r="G86" s="170"/>
-      <c r="H86" s="171"/>
-      <c r="I86" s="171"/>
-      <c r="J86" s="172"/>
+      <c r="G86" s="181"/>
+      <c r="H86" s="182"/>
+      <c r="I86" s="182"/>
+      <c r="J86" s="183"/>
       <c r="K86" s="82"/>
       <c r="L86" s="82"/>
       <c r="M86" s="74"/>
@@ -10289,10 +10617,10 @@
       <c r="D87" s="63"/>
       <c r="E87" s="63"/>
       <c r="F87" s="40"/>
-      <c r="G87" s="170"/>
-      <c r="H87" s="171"/>
-      <c r="I87" s="171"/>
-      <c r="J87" s="172"/>
+      <c r="G87" s="181"/>
+      <c r="H87" s="182"/>
+      <c r="I87" s="182"/>
+      <c r="J87" s="183"/>
       <c r="K87" s="82"/>
       <c r="L87" s="82"/>
       <c r="M87" s="74"/>
@@ -10308,10 +10636,10 @@
       <c r="D88" s="63"/>
       <c r="E88" s="63"/>
       <c r="F88" s="40"/>
-      <c r="G88" s="170"/>
-      <c r="H88" s="171"/>
-      <c r="I88" s="171"/>
-      <c r="J88" s="172"/>
+      <c r="G88" s="181"/>
+      <c r="H88" s="182"/>
+      <c r="I88" s="182"/>
+      <c r="J88" s="183"/>
       <c r="K88" s="82"/>
       <c r="L88" s="82"/>
       <c r="M88" s="74"/>
@@ -10327,10 +10655,10 @@
       <c r="D89" s="63"/>
       <c r="E89" s="63"/>
       <c r="F89" s="40"/>
-      <c r="G89" s="170"/>
-      <c r="H89" s="171"/>
-      <c r="I89" s="171"/>
-      <c r="J89" s="172"/>
+      <c r="G89" s="181"/>
+      <c r="H89" s="182"/>
+      <c r="I89" s="182"/>
+      <c r="J89" s="183"/>
       <c r="K89" s="82"/>
       <c r="L89" s="82"/>
       <c r="M89" s="74"/>
@@ -10346,10 +10674,10 @@
       <c r="D90" s="63"/>
       <c r="E90" s="63"/>
       <c r="F90" s="40"/>
-      <c r="G90" s="170"/>
-      <c r="H90" s="171"/>
-      <c r="I90" s="171"/>
-      <c r="J90" s="172"/>
+      <c r="G90" s="181"/>
+      <c r="H90" s="182"/>
+      <c r="I90" s="182"/>
+      <c r="J90" s="183"/>
       <c r="K90" s="82"/>
       <c r="L90" s="82"/>
       <c r="M90" s="74"/>
@@ -10365,10 +10693,10 @@
       <c r="D91" s="63"/>
       <c r="E91" s="63"/>
       <c r="F91" s="40"/>
-      <c r="G91" s="170"/>
-      <c r="H91" s="171"/>
-      <c r="I91" s="171"/>
-      <c r="J91" s="172"/>
+      <c r="G91" s="181"/>
+      <c r="H91" s="182"/>
+      <c r="I91" s="182"/>
+      <c r="J91" s="183"/>
       <c r="K91" s="82"/>
       <c r="L91" s="82"/>
       <c r="M91" s="74"/>
@@ -10384,10 +10712,10 @@
       <c r="D92" s="63"/>
       <c r="E92" s="63"/>
       <c r="F92" s="40"/>
-      <c r="G92" s="170"/>
-      <c r="H92" s="171"/>
-      <c r="I92" s="171"/>
-      <c r="J92" s="172"/>
+      <c r="G92" s="181"/>
+      <c r="H92" s="182"/>
+      <c r="I92" s="182"/>
+      <c r="J92" s="183"/>
       <c r="K92" s="82"/>
       <c r="L92" s="82"/>
       <c r="M92" s="74"/>
@@ -10403,10 +10731,10 @@
       <c r="D93" s="63"/>
       <c r="E93" s="63"/>
       <c r="F93" s="40"/>
-      <c r="G93" s="170"/>
-      <c r="H93" s="171"/>
-      <c r="I93" s="171"/>
-      <c r="J93" s="172"/>
+      <c r="G93" s="181"/>
+      <c r="H93" s="182"/>
+      <c r="I93" s="182"/>
+      <c r="J93" s="183"/>
       <c r="K93" s="82"/>
       <c r="L93" s="82"/>
       <c r="M93" s="74"/>
@@ -10422,10 +10750,10 @@
       <c r="D94" s="63"/>
       <c r="E94" s="63"/>
       <c r="F94" s="40"/>
-      <c r="G94" s="170"/>
-      <c r="H94" s="171"/>
-      <c r="I94" s="171"/>
-      <c r="J94" s="172"/>
+      <c r="G94" s="181"/>
+      <c r="H94" s="182"/>
+      <c r="I94" s="182"/>
+      <c r="J94" s="183"/>
       <c r="K94" s="82"/>
       <c r="L94" s="82"/>
       <c r="M94" s="74"/>
@@ -10560,8 +10888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -10580,10 +10908,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
+      <c r="B1" s="143"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -10614,8 +10942,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -10892,31 +11220,31 @@
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="72"/>
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="133" t="s">
         <v>209</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="46"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="134"/>
+      <c r="I24" s="134"/>
+      <c r="J24" s="135"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="72"/>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="133" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="46"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
+      <c r="G25" s="134"/>
+      <c r="H25" s="134"/>
+      <c r="I25" s="134"/>
+      <c r="J25" s="135"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="72"/>
@@ -10948,17 +11276,17 @@
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="72"/>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="133" t="s">
         <v>214</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="46"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="134"/>
+      <c r="G28" s="134"/>
+      <c r="H28" s="134"/>
+      <c r="I28" s="134"/>
+      <c r="J28" s="135"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="42"/>
@@ -11735,10 +12063,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
+      <c r="B1" s="143"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -11769,8 +12097,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
+      <c r="A2" s="143"/>
+      <c r="B2" s="143"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -11884,9 +12212,9 @@
       </c>
       <c r="E10" s="125"/>
       <c r="F10" s="123"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="180"/>
+      <c r="G10" s="194"/>
+      <c r="H10" s="194"/>
+      <c r="I10" s="194"/>
       <c r="J10" s="46"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
@@ -11902,9 +12230,9 @@
       </c>
       <c r="E11" s="125"/>
       <c r="F11" s="123"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="180"/>
+      <c r="G11" s="194"/>
+      <c r="H11" s="194"/>
+      <c r="I11" s="194"/>
       <c r="J11" s="46"/>
     </row>
     <row r="12" spans="1:10" ht="11.25">
@@ -11915,16 +12243,16 @@
       <c r="C12" s="124" t="s">
         <v>158</v>
       </c>
-      <c r="D12" s="181" t="s">
+      <c r="D12" s="195" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="182"/>
-      <c r="F12" s="183"/>
-      <c r="G12" s="177" t="s">
+      <c r="E12" s="196"/>
+      <c r="F12" s="197"/>
+      <c r="G12" s="191" t="s">
         <v>160</v>
       </c>
-      <c r="H12" s="178"/>
-      <c r="I12" s="179"/>
+      <c r="H12" s="192"/>
+      <c r="I12" s="193"/>
       <c r="J12" s="46"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
@@ -11935,14 +12263,14 @@
       <c r="C13" s="121" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="174" t="s">
+      <c r="D13" s="188" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="175"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="177"/>
-      <c r="H13" s="178"/>
-      <c r="I13" s="179"/>
+      <c r="E13" s="189"/>
+      <c r="F13" s="190"/>
+      <c r="G13" s="191"/>
+      <c r="H13" s="192"/>
+      <c r="I13" s="193"/>
       <c r="J13" s="46"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
@@ -11958,9 +12286,9 @@
       </c>
       <c r="E14" s="121"/>
       <c r="F14" s="121"/>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="180"/>
+      <c r="G14" s="194"/>
+      <c r="H14" s="194"/>
+      <c r="I14" s="194"/>
       <c r="J14" s="46"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
@@ -11976,9 +12304,9 @@
       </c>
       <c r="E15" s="121"/>
       <c r="F15" s="121"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="180"/>
+      <c r="G15" s="194"/>
+      <c r="H15" s="194"/>
+      <c r="I15" s="194"/>
       <c r="J15" s="46"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
@@ -12225,14 +12553,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25">
-      <c r="B1" s="184" t="s">
+      <c r="B1" s="198" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
+      <c r="C1" s="198"/>
+      <c r="D1" s="198"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1">
       <c r="B2" s="16"/>
@@ -12425,11 +12753,11 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="200.25" customHeight="1">
-      <c r="E27" s="185" t="s">
+      <c r="E27" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="186"/>
-      <c r="G27" s="187"/>
+      <c r="F27" s="200"/>
+      <c r="G27" s="201"/>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="19" t="s">

</xml_diff>